<commit_message>
Updated CSS styling and re-rendered site
</commit_message>
<xml_diff>
--- a/docs/assumptions_and_decision_log_template.xlsx
+++ b/docs/assumptions_and_decision_log_template.xlsx
@@ -4,9 +4,9 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF27A59C-2764-40A6-AD4A-668F784AF0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB232BC8-CC02-470B-A600-81D739BC493E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="405" windowWidth="27300" windowHeight="14160" tabRatio="856" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="11" r:id="rId1"/>
@@ -15,14 +15,14 @@
     <sheet name="Roles and Responsibilities" sheetId="10" r:id="rId4"/>
     <sheet name="R&amp;R Resources" sheetId="12" r:id="rId5"/>
     <sheet name="QA Log" sheetId="14" r:id="rId6"/>
-    <sheet name="Decisions &amp; Issues Register" sheetId="7" r:id="rId7"/>
+    <sheet name="Decisions and Issues Logs" sheetId="7" r:id="rId7"/>
     <sheet name="Assumptions log " sheetId="6" r:id="rId8"/>
     <sheet name="Quality &amp; Sensitivity Guide" sheetId="5" r:id="rId9"/>
     <sheet name="Ethics Log" sheetId="13" r:id="rId10"/>
     <sheet name="Risk Scoring Guide" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Decisions &amp; Issues Register'!$B$10:$L$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Decisions and Issues Logs'!$B$10:$K$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Roles and Responsibilities'!$B$10:$J$11</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="214">
   <si>
     <t>While most of the template should be self explanatory, this introductory slide sets out basic guidance on use.</t>
   </si>
@@ -144,13 +144,7 @@
     <t>QA Log</t>
   </si>
   <si>
-    <t>A Table which allows the Analytical Assurer to document planned Quality Assurance and confirm when it is completed. Also has space for a short summary of the issues the Quality Assurance raised. This information should be described more fully in the decisions and issues register</t>
-  </si>
-  <si>
     <t>Decisions &amp; Issues Register</t>
-  </si>
-  <si>
-    <t>As issues arrise during development, decisions will have to be made about them. These issues do not only arrise from QA, but can be raised frrom within the team. For example, there may be concerns about the validity of one of the inputs used. This requires a decision by the individuals in senior governance positions, who will explain the evidence underpinning this decision. Often these decisions will become assumptions, which are stored in the assumptions log.</t>
   </si>
   <si>
     <t>Assumptions Log</t>
@@ -731,21 +725,12 @@
 Assumption 001 no longer true in view of new evidence</t>
   </si>
   <si>
-    <t>Issues register for [Insert Analysis Name &amp; Financial Year of Interest]</t>
-  </si>
-  <si>
     <t>The decisions log and issues register records the decisions taken by the team and any outstanding issues yet to be addressed.
 Issues can be put on a backlog, but you must explain clearly why this is appropriate (ideally with accompanying evidence) and ensure that the decision to defer the issue is signed off and documented.
 If issues are resolved, they can be evidenced by linking to the relevant place in the analysis where the error, issue or decision impacts.</t>
   </si>
   <si>
     <t>Issue ID</t>
-  </si>
-  <si>
-    <t>Issue</t>
-  </si>
-  <si>
-    <t>Date First Identified</t>
   </si>
   <si>
     <t>Plain English description of issue</t>
@@ -946,9 +931,6 @@
     <t>Most teams will create process maps or model maps during development. These are very helpful to give an overview of the analysis workflow.</t>
   </si>
   <si>
-    <t>This table records the assumptions made about the analysis. Assumptions will often be decisions made because there is a need to simplify the situation in the real world to enable it to be analysed or modelled. Wherever possible, such assumptions should have a numerical value and an uncertainty rangel around the value to demonstrate the uncertainty the team has about the assumption. You should also give your assumptions a quality RAG rating. When this is combined with an assessment about sensitivity of the analysis to the assumption, you get an indicative risk score. Use the risk score to inform how resources are allocated to further research and improvement of the assumptions.</t>
-  </si>
-  <si>
     <t>A at-a-glance guide to quality scoring. If you are not sure about the quality or sensitivity score of an assumption, err on the side of caution and go for lower quality and higher sensitivity.</t>
   </si>
   <si>
@@ -956,13 +938,55 @@
   </si>
   <si>
     <t>This spreadsheet supports analysis development and production by providing a structured template for documentation</t>
+  </si>
+  <si>
+    <t>Decisions Log and Issues register for [Insert Analysis Name &amp; Financial Year of Interest]</t>
+  </si>
+  <si>
+    <t>Issue Name</t>
+  </si>
+  <si>
+    <t>Decision ID</t>
+  </si>
+  <si>
+    <t>Plain English description of decision</t>
+  </si>
+  <si>
+    <t>Decision name</t>
+  </si>
+  <si>
+    <t>Date of Decision</t>
+  </si>
+  <si>
+    <t>Name of person signing off the decision</t>
+  </si>
+  <si>
+    <t>Date Identified</t>
+  </si>
+  <si>
+    <t>Link to issue / risk URL on ONS risk platform</t>
+  </si>
+  <si>
+    <t>Date of next review</t>
+  </si>
+  <si>
+    <t>Role of person signing off the decision</t>
+  </si>
+  <si>
+    <t>A table which allows the Analytical Assurer to document planned Quality Assurance and confirm when it is completed. Also has space for a short summary of the issues the Quality Assurance raised. This information should be described more fully in the decisions and issues register</t>
+  </si>
+  <si>
+    <t>As issues arise in development, decisions will have to be made about them. Issues can come from QA, or be raised from within the team or by stakeholders. For example, there may be concerns about the validity of one of the inputs used. This requires a decision by the individuals in senior governance positions, who will explain the evidence underpinning this decision. Often these decisions will become assumptions, which are stored in the assumptions log.</t>
+  </si>
+  <si>
+    <t>This table records the assumptions made about the analysis. Assumptions will often be decisions made because there is a need to simplify the real world so it can be analysed or modelled. Wherever possible, such assumptions should have a numerical value and an uncertainty range around the value. You should also give your assumptions a quality RAG rating. When this is combined with an assessment about how sensitive the analysis is to the assumption, you get an indicative risk score. Use the risk score to inform how resources are allocated to further research and improvement of the assumptions.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1129,8 +1153,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1183,6 +1214,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1592,7 +1635,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1922,6 +1965,21 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2750,40 +2808,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0E718D-ABA6-478B-BFB8-19647D312746}">
   <dimension ref="B2:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="45"/>
-    <col min="2" max="2" width="15.6640625" style="80" customWidth="1"/>
-    <col min="3" max="3" width="94.33203125" style="52" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="45"/>
+    <col min="2" max="2" width="15.7109375" style="80" customWidth="1"/>
+    <col min="3" max="3" width="94.28515625" style="52" customWidth="1"/>
     <col min="4" max="4" width="39" style="45" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="45"/>
+    <col min="5" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="99" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="99" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="99" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="99" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="56" t="s">
         <v>3</v>
       </c>
@@ -2791,19 +2849,19 @@
         <v>4</v>
       </c>
       <c r="D7" s="56" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="56" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="79" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D8" s="79"/>
     </row>
-    <row r="9" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="56" t="s">
         <v>6</v>
       </c>
@@ -2812,7 +2870,7 @@
       </c>
       <c r="D9" s="79"/>
     </row>
-    <row r="10" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="56" t="s">
         <v>8</v>
       </c>
@@ -2823,7 +2881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="56" t="s">
         <v>11</v>
       </c>
@@ -2832,69 +2890,69 @@
       </c>
       <c r="D11" s="79"/>
     </row>
-    <row r="12" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="56" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="79" t="s">
+        <v>211</v>
+      </c>
+      <c r="D12" s="79"/>
+    </row>
+    <row r="13" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B13" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="79"/>
-    </row>
-    <row r="13" spans="2:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="B13" s="54" t="s">
+      <c r="C13" s="81" t="s">
+        <v>212</v>
+      </c>
+      <c r="D13" s="81"/>
+    </row>
+    <row r="14" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="B14" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="81" t="s">
+      <c r="C14" s="79" t="s">
+        <v>213</v>
+      </c>
+      <c r="D14" s="79"/>
+    </row>
+    <row r="15" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="81"/>
-    </row>
-    <row r="14" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="56" t="s">
+      <c r="C15" s="79" t="s">
+        <v>197</v>
+      </c>
+      <c r="D15" s="79"/>
+    </row>
+    <row r="16" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="79" t="s">
-        <v>202</v>
-      </c>
-      <c r="D14" s="79"/>
-    </row>
-    <row r="15" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="56" t="s">
+      <c r="C16" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="79" t="s">
-        <v>203</v>
-      </c>
-      <c r="D15" s="79"/>
-    </row>
-    <row r="16" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="79" t="s">
-        <v>20</v>
-      </c>
       <c r="D16" s="79"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="80"/>
       <c r="D17" s="80"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="80"/>
       <c r="D18" s="80"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D19" s="52"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D20" s="52"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D21" s="52"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D22" s="52"/>
     </row>
   </sheetData>
@@ -2913,21 +2971,21 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="88" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2949,115 +3007,115 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="1"/>
-    <col min="2" max="2" width="42.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="1.5546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="42.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="1.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="48.9" customHeight="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="34"/>
       <c r="E7" s="35"/>
       <c r="F7" s="35"/>
       <c r="G7" s="35"/>
       <c r="H7" s="36" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I7" s="35"/>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="2:10" ht="6.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="6.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="37"/>
       <c r="J8" s="26"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D9" s="38"/>
       <c r="G9" s="29" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H9" s="29" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="J9" s="26"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D10" s="38"/>
       <c r="F10" s="28" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I10" s="33" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="J10" s="26"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D11" s="39" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G11" s="33" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H11" s="33" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="I11" s="33" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="J11" s="26"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D12" s="38"/>
       <c r="F12" s="28" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="I12" s="33" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="J12" s="26"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D13" s="31"/>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
@@ -3066,14 +3124,14 @@
       <c r="I13" s="27"/>
       <c r="J13" s="30"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -3092,163 +3150,163 @@
       <selection activeCell="D26" sqref="A1:D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="45"/>
-    <col min="2" max="2" width="23.5546875" style="53" customWidth="1"/>
-    <col min="3" max="3" width="72.88671875" style="45" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="97.44140625" style="45" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="45"/>
+    <col min="1" max="1" width="9.140625" style="45"/>
+    <col min="2" max="2" width="23.5703125" style="53" customWidth="1"/>
+    <col min="3" max="3" width="72.85546875" style="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="97.42578125" style="45" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="C2" s="49"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="55" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="54" t="s">
+      <c r="C3" s="50"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="49"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="55" t="s">
+      <c r="C4" s="50"/>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="55" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="50"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="50"/>
-    </row>
-    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B5" s="55" t="s">
-        <v>26</v>
       </c>
       <c r="C5" s="50"/>
       <c r="D5" s="52" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="48"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="46" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="56" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="48"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="46" t="s">
+      <c r="C9" s="49"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="56" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="54" t="s">
+      <c r="C10" s="47"/>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="49"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="56" t="s">
+      <c r="C11" s="51"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="47"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="57" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B14" s="56" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" s="51"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="46" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="56" t="s">
-        <v>34</v>
       </c>
       <c r="C14" s="48"/>
       <c r="D14" s="58" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="56" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C15" s="48"/>
       <c r="D15" s="58" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="56" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" s="48"/>
       <c r="D16" s="58" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="46"/>
       <c r="B19" s="54" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" s="50"/>
       <c r="D19" s="98" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="46"/>
       <c r="B20" s="54" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" s="50"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="56" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C21" s="48"/>
       <c r="D21" s="98" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="53"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="56" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="46" t="s">
+      <c r="C24" s="48"/>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="53"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="56" t="s">
+      <c r="C25" s="50"/>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="56" t="s">
         <v>47</v>
-      </c>
-      <c r="C24" s="48"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="50"/>
-    </row>
-    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B26" s="56" t="s">
-        <v>49</v>
       </c>
       <c r="C26" s="48"/>
     </row>
@@ -3272,217 +3330,217 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="45"/>
-    <col min="2" max="2" width="27.109375" style="77" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="45" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" style="45" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" style="45" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" style="52" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="45"/>
-    <col min="8" max="8" width="38.109375" style="45" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="45"/>
+    <col min="1" max="1" width="9.140625" style="45"/>
+    <col min="2" max="2" width="27.140625" style="77" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="45" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="45" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="52" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="45"/>
+    <col min="8" max="8" width="38.140625" style="45" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="76"/>
     </row>
-    <row r="2" spans="1:8" s="75" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="74"/>
       <c r="B2" s="89" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D2" s="74"/>
       <c r="F2" s="78"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="89" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="89" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="91" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="89" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="91" t="s">
+      <c r="C7" s="45" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="45" t="s">
+    <row r="8" spans="1:8" s="74" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="D8" s="74" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="74" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="53" t="s">
+      <c r="F8" s="90" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="74" t="s">
+      <c r="H8" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="90" t="s">
-        <v>57</v>
-      </c>
-      <c r="H8" s="74" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="46"/>
       <c r="B10" s="95" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="45"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="93" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="45"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="93" t="s">
+      <c r="F11" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="H11" s="97" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="45" t="s">
+    </row>
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="94" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="97" t="s">
+      <c r="D12" s="45" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="94" t="s">
+      <c r="F12" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="H12" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="F12" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="96" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="91"/>
       <c r="F13" s="45"/>
       <c r="H13" s="96" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="91"/>
       <c r="F14" s="45"/>
       <c r="H14" s="96" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="46"/>
       <c r="B15" s="95" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F15" s="45"/>
       <c r="H15" s="96"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="93" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D16" s="92"/>
       <c r="F16" s="45"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="93" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D17" s="92"/>
       <c r="F17" s="45"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="91"/>
       <c r="D18" s="92"/>
       <c r="F18" s="45"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="91"/>
       <c r="F19" s="45"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="91"/>
       <c r="F20" s="45"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="45"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="91" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" s="45"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="91" t="s">
-        <v>75</v>
-      </c>
       <c r="F22" s="45"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="91"/>
       <c r="F23" s="45"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="46"/>
       <c r="B24" s="91"/>
       <c r="F24" s="45"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
       <c r="B25" s="91"/>
       <c r="F25" s="45"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="91"/>
       <c r="F26" s="45"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="91"/>
       <c r="F27" s="45"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="91"/>
       <c r="F28" s="45"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="91"/>
       <c r="F29" s="45"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="91"/>
       <c r="F30" s="45"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="91"/>
       <c r="F31" s="45"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="91"/>
       <c r="F32" s="45"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="91"/>
       <c r="F33" s="45"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="91"/>
       <c r="F34" s="45"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="91"/>
       <c r="F35" s="45"/>
     </row>
@@ -3503,30 +3561,30 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="24.44140625" style="42" customWidth="1"/>
-    <col min="3" max="4" width="16.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="58.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="29.33203125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="24.42578125" style="42" customWidth="1"/>
+    <col min="3" max="4" width="16.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="58.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
     </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="6"/>
@@ -3537,7 +3595,7 @@
       <c r="J2" s="13"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -3550,10 +3608,10 @@
       <c r="J3" s="13"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="111" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" s="112"/>
       <c r="D4" s="112"/>
@@ -3565,7 +3623,7 @@
       <c r="J4" s="13"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="113"/>
       <c r="C5" s="114"/>
@@ -3578,7 +3636,7 @@
       <c r="J5" s="13"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="113"/>
       <c r="C6" s="114"/>
@@ -3591,7 +3649,7 @@
       <c r="J6" s="13"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="115"/>
       <c r="C7" s="116"/>
@@ -3604,7 +3662,7 @@
       <c r="J7" s="13"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3617,44 +3675,44 @@
       <c r="J8" s="13"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="G10" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="H10" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="I10" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I10" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -3666,10 +3724,10 @@
       <c r="J11" s="14"/>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="43" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -3681,9 +3739,9 @@
       <c r="J12" s="15"/>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="44" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
@@ -3694,17 +3752,17 @@
       <c r="I13" s="41"/>
       <c r="J13" s="41"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -3715,9 +3773,9 @@
       <c r="I16" s="15"/>
       <c r="J16" s="14"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="43" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -3728,9 +3786,9 @@
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="44" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C18" s="41"/>
       <c r="D18" s="41"/>
@@ -3766,198 +3824,198 @@
       <selection sqref="A1:N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" style="62" customWidth="1"/>
-    <col min="2" max="2" width="103.33203125" style="62" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="62" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.109375" style="62"/>
+    <col min="1" max="1" width="18.85546875" style="62" customWidth="1"/>
+    <col min="2" max="2" width="103.28515625" style="62" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="62" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="62"/>
     <col min="6" max="6" width="30" style="62" customWidth="1"/>
-    <col min="7" max="7" width="71.5546875" style="59" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" style="62" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.109375" style="62"/>
+    <col min="7" max="7" width="71.5703125" style="59" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" style="62" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="62"/>
     <col min="11" max="11" width="30" style="62" customWidth="1"/>
-    <col min="12" max="12" width="97.5546875" style="62" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" style="62" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="62"/>
+    <col min="12" max="12" width="97.5703125" style="62" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="62" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="61"/>
+    </row>
+    <row r="4" spans="1:14" ht="87.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="100" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="B4" s="102" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="61"/>
-    </row>
-    <row r="4" spans="1:14" ht="69" x14ac:dyDescent="0.25">
-      <c r="A4" s="100" t="s">
+      <c r="F4" s="101" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="102" t="s">
+      <c r="G4" s="103" t="s">
         <v>94</v>
-      </c>
-      <c r="F4" s="101" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" s="103" t="s">
-        <v>96</v>
       </c>
       <c r="H4" s="73"/>
       <c r="I4" s="73"/>
       <c r="J4" s="73"/>
       <c r="K4" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="L4" s="103" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="61"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="61"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="72" t="s">
         <v>97</v>
       </c>
-      <c r="L4" s="103" t="s">
+      <c r="F7" s="72" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="61"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="61"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
-        <v>99</v>
-      </c>
-      <c r="F7" s="72" t="s">
-        <v>100</v>
       </c>
       <c r="G7" s="66"/>
       <c r="K7" s="65" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="65" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="67" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="67" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" s="65" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="67" t="s">
+      <c r="D8" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="67" t="s">
+      <c r="G8" s="67" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="I8" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="L8" s="67" t="s">
+        <v>100</v>
+      </c>
+      <c r="M8" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="N8" s="67" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="B9" s="60" t="s">
         <v>103</v>
-      </c>
-      <c r="D8" s="67" t="s">
-        <v>104</v>
-      </c>
-      <c r="G8" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="H8" s="67" t="s">
-        <v>103</v>
-      </c>
-      <c r="I8" s="67" t="s">
-        <v>104</v>
-      </c>
-      <c r="L8" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="M8" s="67" t="s">
-        <v>103</v>
-      </c>
-      <c r="N8" s="67" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="B9" s="60" t="s">
-        <v>105</v>
       </c>
       <c r="C9" s="69"/>
       <c r="D9" s="69"/>
       <c r="G9" s="104" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H9" s="69"/>
       <c r="I9" s="69"/>
       <c r="L9" s="104" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M9" s="69"/>
       <c r="N9" s="69"/>
     </row>
-    <row r="10" spans="1:14" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B10" s="60" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C10" s="69"/>
       <c r="D10" s="69"/>
       <c r="G10" s="70" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H10" s="69"/>
       <c r="I10" s="69"/>
       <c r="L10" s="104" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M10" s="69"/>
       <c r="N10" s="69"/>
     </row>
-    <row r="11" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B11" s="60" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C11" s="69"/>
       <c r="D11" s="69"/>
       <c r="G11" s="104" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H11" s="69"/>
       <c r="I11" s="69"/>
       <c r="L11" s="70" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M11" s="69"/>
       <c r="N11" s="69"/>
     </row>
-    <row r="12" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B12" s="60" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C12" s="69"/>
       <c r="D12" s="69"/>
       <c r="G12" s="104" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H12" s="69"/>
       <c r="I12" s="69"/>
       <c r="L12" s="104" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M12" s="69"/>
       <c r="N12" s="69"/>
     </row>
-    <row r="13" spans="1:14" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B13" s="60" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C13" s="69"/>
       <c r="D13" s="69"/>
       <c r="G13" s="105" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H13" s="69"/>
       <c r="I13" s="69"/>
       <c r="L13" s="60" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="M13" s="69"/>
       <c r="N13" s="69"/>
     </row>
-    <row r="14" spans="1:14" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="44.25" x14ac:dyDescent="0.25">
       <c r="B14" s="71" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C14" s="69"/>
       <c r="D14" s="69"/>
       <c r="G14" s="105" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H14" s="69"/>
       <c r="I14" s="69"/>
@@ -3965,48 +4023,48 @@
       <c r="M14" s="69"/>
       <c r="N14" s="69"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="65" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" s="65" t="s">
+        <v>121</v>
+      </c>
+      <c r="K16" s="65" t="s">
         <v>122</v>
       </c>
-      <c r="F16" s="65" t="s">
+    </row>
+    <row r="17" spans="7:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="G17" s="68" t="s">
         <v>123</v>
       </c>
-      <c r="K16" s="65" t="s">
+      <c r="H17" s="67" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="17" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G17" s="68" t="s">
+      <c r="I17" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="L17" s="67" t="s">
         <v>125</v>
       </c>
-      <c r="H17" s="67" t="s">
+      <c r="M17" s="67" t="s">
+        <v>124</v>
+      </c>
+      <c r="N17" s="67" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="7:14" ht="100.5" x14ac:dyDescent="0.2">
+      <c r="G18" s="106" t="s">
         <v>126</v>
-      </c>
-      <c r="I17" s="67" t="s">
-        <v>104</v>
-      </c>
-      <c r="L17" s="67" t="s">
-        <v>127</v>
-      </c>
-      <c r="M17" s="67" t="s">
-        <v>126</v>
-      </c>
-      <c r="N17" s="67" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="7:14" ht="82.8" x14ac:dyDescent="0.25">
-      <c r="G18" s="106" t="s">
-        <v>128</v>
       </c>
       <c r="H18" s="69"/>
       <c r="I18" s="69"/>
       <c r="J18" s="62" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L18" s="106" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M18" s="69"/>
       <c r="N18" s="69"/>
@@ -4030,34 +4088,34 @@
       <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="65.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="70.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="65.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="70.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="42" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.44140625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" style="12" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" s="6" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="D2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="111" t="s">
         <v>131</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="H2" s="13"/>
-    </row>
-    <row r="3" spans="1:8" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="H3" s="13"/>
-    </row>
-    <row r="4" spans="1:8" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="111" t="s">
-        <v>133</v>
       </c>
       <c r="C4" s="117"/>
       <c r="D4" s="112"/>
@@ -4066,7 +4124,7 @@
       <c r="G4" s="118"/>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="113"/>
       <c r="C5" s="114"/>
       <c r="D5" s="114"/>
@@ -4075,7 +4133,7 @@
       <c r="G5" s="119"/>
       <c r="H5" s="13"/>
     </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="113"/>
       <c r="C6" s="114"/>
       <c r="D6" s="114"/>
@@ -4084,7 +4142,7 @@
       <c r="G6" s="119"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="115"/>
       <c r="C7" s="116"/>
       <c r="D7" s="116"/>
@@ -4093,150 +4151,150 @@
       <c r="G7" s="120"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="G10" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="H10" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" s="9" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="10">
         <v>1</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="F11" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="G11" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>145</v>
-      </c>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="H12" s="19"/>
     </row>
-    <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="H13" s="19"/>
     </row>
-    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="H14" s="19"/>
     </row>
-    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="4:8" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:8" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H20" s="20"/>
     </row>
-    <row r="21" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H21" s="20"/>
     </row>
-    <row r="22" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H22" s="20"/>
     </row>
-    <row r="23" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H23" s="20"/>
     </row>
-    <row r="24" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H24" s="20"/>
     </row>
-    <row r="25" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H25" s="20"/>
     </row>
-    <row r="26" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H26" s="20"/>
     </row>
-    <row r="27" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H27" s="20"/>
     </row>
-    <row r="28" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H28" s="20"/>
     </row>
-    <row r="29" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H29" s="20"/>
     </row>
-    <row r="30" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H30" s="20"/>
     </row>
-    <row r="31" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H31" s="20"/>
     </row>
-    <row r="32" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H32" s="20"/>
     </row>
-    <row r="33" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H33" s="20"/>
     </row>
-    <row r="34" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H34" s="20"/>
     </row>
-    <row r="35" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H35" s="20"/>
     </row>
-    <row r="36" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H36" s="20"/>
     </row>
   </sheetData>
@@ -4257,44 +4315,47 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.6640625" style="1"/>
-    <col min="3" max="4" width="16.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="58.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="30.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="29.33203125" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19" style="1" customWidth="1"/>
+    <col min="11" max="11" width="26.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22" style="1" customWidth="1"/>
+    <col min="13" max="13" width="50.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
-        <v>146</v>
+        <v>200</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I2" s="24"/>
       <c r="J2" s="13"/>
@@ -4302,7 +4363,7 @@
       <c r="L2" s="13"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -4317,10 +4378,10 @@
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="121" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C4" s="122"/>
       <c r="D4" s="122"/>
@@ -4334,7 +4395,7 @@
       <c r="L4" s="13"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="124"/>
       <c r="C5" s="114"/>
@@ -4349,7 +4410,7 @@
       <c r="L5" s="13"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="124"/>
       <c r="C6" s="114"/>
@@ -4364,7 +4425,7 @@
       <c r="L6" s="13"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="126"/>
       <c r="C7" s="127"/>
@@ -4379,7 +4440,7 @@
       <c r="L7" s="13"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="16"/>
       <c r="C8" s="6"/>
@@ -4394,212 +4455,386 @@
       <c r="L8" s="13"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
+    <row r="10" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="134" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="134" t="s">
+        <v>201</v>
+      </c>
+      <c r="D10" s="134" t="s">
+        <v>207</v>
+      </c>
+      <c r="E10" s="134" t="s">
+        <v>146</v>
+      </c>
+      <c r="F10" s="134" t="s">
+        <v>147</v>
+      </c>
+      <c r="G10" s="134" t="s">
         <v>148</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="H10" s="134" t="s">
         <v>149</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="I10" s="134" t="s">
         <v>150</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="J10" s="134" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" s="134" t="s">
         <v>151</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L10" s="134" t="s">
+        <v>209</v>
+      </c>
+      <c r="M10" s="136" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
-      <c r="B11" s="10"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I11" s="137"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="137"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="138"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="9"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="41"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="41"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
+      <c r="I12" s="137"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="138"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="138"/>
+      <c r="C13" s="138"/>
+      <c r="D13" s="138"/>
+      <c r="E13" s="138"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="138"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="138"/>
+      <c r="J13" s="138"/>
+      <c r="K13" s="138"/>
+      <c r="L13" s="138"/>
+      <c r="M13" s="138"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="138"/>
+      <c r="C14" s="138"/>
+      <c r="D14" s="138"/>
+      <c r="E14" s="138"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="138"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="138"/>
+      <c r="J14" s="138"/>
+      <c r="K14" s="138"/>
+      <c r="L14" s="138"/>
+      <c r="M14" s="138"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="138"/>
+      <c r="C15" s="138"/>
+      <c r="D15" s="138"/>
+      <c r="E15" s="138"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="138"/>
+      <c r="H15" s="138"/>
+      <c r="I15" s="138"/>
+      <c r="J15" s="138"/>
+      <c r="K15" s="138"/>
+      <c r="L15" s="138"/>
+      <c r="M15" s="138"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="138"/>
+      <c r="C16" s="138"/>
+      <c r="D16" s="138"/>
+      <c r="E16" s="138"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="138"/>
+      <c r="H16" s="138"/>
+      <c r="I16" s="138"/>
+      <c r="J16" s="138"/>
+      <c r="K16" s="138"/>
+      <c r="L16" s="138"/>
+      <c r="M16" s="138"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="138"/>
+      <c r="C17" s="138"/>
+      <c r="D17" s="138"/>
+      <c r="E17" s="138"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="138"/>
+      <c r="H17" s="138"/>
+      <c r="I17" s="138"/>
+      <c r="J17" s="138"/>
+      <c r="K17" s="138"/>
+      <c r="L17" s="138"/>
+      <c r="M17" s="138"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="138"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="138"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="138"/>
+      <c r="H18" s="138"/>
+      <c r="I18" s="138"/>
+      <c r="J18" s="138"/>
+      <c r="K18" s="138"/>
+      <c r="L18" s="138"/>
+      <c r="M18" s="138"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="138"/>
+      <c r="C19" s="138"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="138"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="138"/>
+      <c r="H19" s="138"/>
+      <c r="I19" s="138"/>
+      <c r="J19" s="138"/>
+      <c r="K19" s="138"/>
+      <c r="L19" s="138"/>
+      <c r="M19" s="138"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="138"/>
+      <c r="C20" s="138"/>
+      <c r="D20" s="138"/>
+      <c r="E20" s="138"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="138"/>
+      <c r="H20" s="138"/>
+      <c r="I20" s="138"/>
+      <c r="J20" s="138"/>
+      <c r="K20" s="138"/>
+      <c r="L20" s="138"/>
+      <c r="M20" s="138"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="138"/>
+      <c r="C21" s="138"/>
+      <c r="D21" s="138"/>
+      <c r="E21" s="138"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="138"/>
+      <c r="H21" s="138"/>
+      <c r="I21" s="138"/>
+      <c r="J21" s="138"/>
+      <c r="K21" s="138"/>
+      <c r="L21" s="138"/>
+      <c r="M21" s="138"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="138"/>
+      <c r="C22" s="138"/>
+      <c r="D22" s="138"/>
+      <c r="E22" s="138"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="138"/>
+      <c r="H22" s="138"/>
+      <c r="I22" s="138"/>
+      <c r="J22" s="138"/>
+      <c r="K22" s="138"/>
+      <c r="L22" s="138"/>
+      <c r="M22" s="138"/>
+    </row>
+    <row r="25" spans="2:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="135" t="s">
+        <v>202</v>
+      </c>
+      <c r="C25" s="135" t="s">
+        <v>204</v>
+      </c>
+      <c r="D25" s="135" t="s">
+        <v>203</v>
+      </c>
+      <c r="E25" s="135" t="s">
+        <v>205</v>
+      </c>
+      <c r="F25" s="135" t="s">
+        <v>206</v>
+      </c>
+      <c r="G25" s="135" t="s">
+        <v>210</v>
+      </c>
+      <c r="H25" s="135" t="s">
+        <v>82</v>
+      </c>
+      <c r="I25" s="135" t="s">
+        <v>151</v>
+      </c>
+      <c r="J25" s="135" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="82"/>
+      <c r="I26" s="137"/>
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="138"/>
+      <c r="C28" s="138"/>
+      <c r="D28" s="138"/>
+      <c r="E28" s="138"/>
+      <c r="F28" s="138"/>
+      <c r="G28" s="138"/>
+      <c r="H28" s="138"/>
+      <c r="I28" s="138"/>
+      <c r="J28" s="138"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="138"/>
+      <c r="C29" s="138"/>
+      <c r="D29" s="138"/>
+      <c r="E29" s="138"/>
+      <c r="F29" s="138"/>
+      <c r="G29" s="138"/>
+      <c r="H29" s="138"/>
+      <c r="I29" s="138"/>
+      <c r="J29" s="138"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="138"/>
+      <c r="C30" s="138"/>
+      <c r="D30" s="138"/>
+      <c r="E30" s="138"/>
+      <c r="F30" s="138"/>
+      <c r="G30" s="138"/>
+      <c r="H30" s="138"/>
+      <c r="I30" s="138"/>
+      <c r="J30" s="138"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="138"/>
+      <c r="C31" s="138"/>
+      <c r="D31" s="138"/>
+      <c r="E31" s="138"/>
+      <c r="F31" s="138"/>
+      <c r="G31" s="138"/>
+      <c r="H31" s="138"/>
+      <c r="I31" s="138"/>
+      <c r="J31" s="138"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="138"/>
+      <c r="C32" s="138"/>
+      <c r="D32" s="138"/>
+      <c r="E32" s="138"/>
+      <c r="F32" s="138"/>
+      <c r="G32" s="138"/>
+      <c r="H32" s="138"/>
+      <c r="I32" s="138"/>
+      <c r="J32" s="138"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="138"/>
+      <c r="C33" s="138"/>
+      <c r="D33" s="138"/>
+      <c r="E33" s="138"/>
+      <c r="F33" s="138"/>
+      <c r="G33" s="138"/>
+      <c r="H33" s="138"/>
+      <c r="I33" s="138"/>
+      <c r="J33" s="138"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="138"/>
+      <c r="C34" s="138"/>
+      <c r="D34" s="138"/>
+      <c r="E34" s="138"/>
+      <c r="F34" s="138"/>
+      <c r="G34" s="138"/>
+      <c r="H34" s="138"/>
+      <c r="I34" s="138"/>
+      <c r="J34" s="138"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="138"/>
+      <c r="C35" s="138"/>
+      <c r="D35" s="138"/>
+      <c r="E35" s="138"/>
+      <c r="F35" s="138"/>
+      <c r="G35" s="138"/>
+      <c r="H35" s="138"/>
+      <c r="I35" s="138"/>
+      <c r="J35" s="138"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="138"/>
+      <c r="C36" s="138"/>
+      <c r="D36" s="138"/>
+      <c r="E36" s="138"/>
+      <c r="F36" s="138"/>
+      <c r="G36" s="138"/>
+      <c r="H36" s="138"/>
+      <c r="I36" s="138"/>
+      <c r="J36" s="138"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="138"/>
+      <c r="C37" s="138"/>
+      <c r="D37" s="138"/>
+      <c r="E37" s="138"/>
+      <c r="F37" s="138"/>
+      <c r="G37" s="138"/>
+      <c r="H37" s="138"/>
+      <c r="I37" s="138"/>
+      <c r="J37" s="138"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B4:H7"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G11:G22" xr:uid="{725DA519-1BD3-441D-A0B8-12DB83D680BE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:F22" xr:uid="{725DA519-1BD3-441D-A0B8-12DB83D680BE}">
       <formula1>"Resolved, Shelved"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4621,33 +4856,33 @@
       <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="65.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="53.109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="38.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="65.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="53.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="38.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="26" style="1" customWidth="1"/>
     <col min="11" max="11" width="15" style="12" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" style="12" customWidth="1"/>
-    <col min="13" max="16" width="17.33203125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="12" customWidth="1"/>
+    <col min="13" max="16" width="17.28515625" style="12" customWidth="1"/>
     <col min="17" max="17" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" s="6" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:19" s="6" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="D2" s="7" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
@@ -4656,7 +4891,7 @@
       <c r="O2" s="13"/>
       <c r="P2" s="13"/>
     </row>
-    <row r="3" spans="1:19" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
@@ -4664,9 +4899,9 @@
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
     </row>
-    <row r="4" spans="1:19" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="111" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C4" s="117"/>
       <c r="D4" s="112"/>
@@ -4683,7 +4918,7 @@
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
     </row>
-    <row r="5" spans="1:19" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="113"/>
       <c r="C5" s="114"/>
       <c r="D5" s="114"/>
@@ -4700,7 +4935,7 @@
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
     </row>
-    <row r="6" spans="1:19" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="113"/>
       <c r="C6" s="114"/>
       <c r="D6" s="114"/>
@@ -4717,7 +4952,7 @@
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
     </row>
-    <row r="7" spans="1:19" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="115"/>
       <c r="C7" s="116"/>
       <c r="D7" s="116"/>
@@ -4734,7 +4969,7 @@
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
-    <row r="8" spans="1:19" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="K8" s="13"/>
@@ -4744,63 +4979,63 @@
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
     </row>
-    <row r="10" spans="1:19" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="H10" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="I10" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="K10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="M10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="N10" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="O10" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="P10" s="84" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q10" s="86" t="s">
         <v>166</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="R10" s="86" t="s">
         <v>167</v>
       </c>
-      <c r="K10" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="L10" s="8" t="s">
+      <c r="S10" s="86" t="s">
         <v>168</v>
       </c>
-      <c r="M10" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="O10" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="P10" s="84" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q10" s="86" t="s">
-        <v>171</v>
-      </c>
-      <c r="R10" s="86" t="s">
-        <v>172</v>
-      </c>
-      <c r="S10" s="86" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" s="9" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:19" s="9" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="10">
         <v>1</v>
@@ -4820,16 +5055,16 @@
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
       <c r="Q11" s="85" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="R11" s="87" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="S11" s="87" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
@@ -4844,7 +5079,7 @@
       <c r="P12" s="20"/>
       <c r="Q12" s="22"/>
     </row>
-    <row r="13" spans="1:19" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
@@ -4859,7 +5094,7 @@
       <c r="P13" s="20"/>
       <c r="Q13" s="22"/>
     </row>
-    <row r="14" spans="1:19" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
@@ -4874,7 +5109,7 @@
       <c r="P14" s="20"/>
       <c r="Q14" s="21"/>
     </row>
-    <row r="15" spans="1:19" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
@@ -4889,7 +5124,7 @@
       <c r="P15" s="20"/>
       <c r="Q15" s="21"/>
     </row>
-    <row r="16" spans="1:19" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
@@ -4904,7 +5139,7 @@
       <c r="P16" s="20"/>
       <c r="Q16" s="21"/>
     </row>
-    <row r="17" spans="4:17" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:17" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
@@ -4919,7 +5154,7 @@
       <c r="P17" s="20"/>
       <c r="Q17" s="21"/>
     </row>
-    <row r="18" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
@@ -4934,7 +5169,7 @@
       <c r="P18" s="20"/>
       <c r="Q18" s="21"/>
     </row>
-    <row r="19" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K19" s="20"/>
       <c r="L19" s="20"/>
       <c r="M19" s="20"/>
@@ -4943,7 +5178,7 @@
       <c r="P19" s="20"/>
       <c r="Q19" s="22"/>
     </row>
-    <row r="20" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -4952,7 +5187,7 @@
       <c r="P20" s="20"/>
       <c r="Q20" s="22"/>
     </row>
-    <row r="21" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
@@ -4961,7 +5196,7 @@
       <c r="P21" s="20"/>
       <c r="Q21" s="22"/>
     </row>
-    <row r="22" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
@@ -4970,7 +5205,7 @@
       <c r="P22" s="20"/>
       <c r="Q22" s="22"/>
     </row>
-    <row r="23" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
       <c r="M23" s="20"/>
@@ -4979,7 +5214,7 @@
       <c r="P23" s="20"/>
       <c r="Q23" s="22"/>
     </row>
-    <row r="24" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
@@ -4988,7 +5223,7 @@
       <c r="P24" s="20"/>
       <c r="Q24" s="22"/>
     </row>
-    <row r="25" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K25" s="20"/>
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
@@ -4997,7 +5232,7 @@
       <c r="P25" s="20"/>
       <c r="Q25" s="22"/>
     </row>
-    <row r="26" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
@@ -5006,7 +5241,7 @@
       <c r="P26" s="20"/>
       <c r="Q26" s="22"/>
     </row>
-    <row r="27" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K27" s="20"/>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
@@ -5015,7 +5250,7 @@
       <c r="P27" s="20"/>
       <c r="Q27" s="22"/>
     </row>
-    <row r="28" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K28" s="20"/>
       <c r="L28" s="20"/>
       <c r="M28" s="20"/>
@@ -5024,7 +5259,7 @@
       <c r="P28" s="20"/>
       <c r="Q28" s="22"/>
     </row>
-    <row r="29" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K29" s="20"/>
       <c r="L29" s="20"/>
       <c r="M29" s="20"/>
@@ -5033,7 +5268,7 @@
       <c r="P29" s="20"/>
       <c r="Q29" s="22"/>
     </row>
-    <row r="30" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K30" s="20"/>
       <c r="L30" s="20"/>
       <c r="M30" s="20"/>
@@ -5042,7 +5277,7 @@
       <c r="P30" s="20"/>
       <c r="Q30" s="22"/>
     </row>
-    <row r="31" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K31" s="20"/>
       <c r="L31" s="20"/>
       <c r="M31" s="20"/>
@@ -5051,7 +5286,7 @@
       <c r="P31" s="20"/>
       <c r="Q31" s="22"/>
     </row>
-    <row r="32" spans="4:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
       <c r="M32" s="20"/>
@@ -5060,7 +5295,7 @@
       <c r="P32" s="20"/>
       <c r="Q32" s="22"/>
     </row>
-    <row r="33" spans="11:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K33" s="20"/>
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
@@ -5069,7 +5304,7 @@
       <c r="P33" s="20"/>
       <c r="Q33" s="22"/>
     </row>
-    <row r="34" spans="11:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
       <c r="M34" s="20"/>
@@ -5078,7 +5313,7 @@
       <c r="P34" s="20"/>
       <c r="Q34" s="22"/>
     </row>
-    <row r="35" spans="11:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
       <c r="M35" s="20"/>
@@ -5087,7 +5322,7 @@
       <c r="P35" s="20"/>
       <c r="Q35" s="22"/>
     </row>
-    <row r="36" spans="11:17" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K36" s="20"/>
       <c r="L36" s="20"/>
       <c r="M36" s="20"/>
@@ -5136,94 +5371,94 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="30" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="26.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="42.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="42.85546875" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="138.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="129" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C2" s="109" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" s="132" t="s">
         <v>174</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="F2" s="132" t="s">
-        <v>179</v>
-      </c>
       <c r="G2" s="110" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H2" s="83" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="144.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="130"/>
       <c r="C3" s="108" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="133"/>
       <c r="G3" s="110" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H3" s="83" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="121.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="131"/>
       <c r="C4" s="107" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F4" s="133"/>
       <c r="G4" s="110" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="H4" s="83" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="F7" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
     </row>
   </sheetData>
@@ -5240,12 +5475,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e1cd103-0302-4a32-9a4b-e115c950d959">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5492,20 +5729,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e1cd103-0302-4a32-9a4b-e115c950d959">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D186559C-C381-484C-9B7A-F4466E79AE25}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71C399E-D560-405D-A693-6A86DF1C82D7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4"/>
+    <ds:schemaRef ds:uri="7e1cd103-0302-4a32-9a4b-e115c950d959"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5530,18 +5774,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71C399E-D560-405D-A693-6A86DF1C82D7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D186559C-C381-484C-9B7A-F4466E79AE25}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4"/>
-    <ds:schemaRef ds:uri="7e1cd103-0302-4a32-9a4b-e115c950d959"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Re-rendered website to incorporate revised Excel sheet
</commit_message>
<xml_diff>
--- a/docs/assumptions_and_decision_log_template.xlsx
+++ b/docs/assumptions_and_decision_log_template.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27417"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15C39A0E-A134-4DE1-858E-D7C6F615B827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1010" documentId="8_{C66C9284-12B1-4C2F-AAEC-29ECF8510037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21B1B33D-F6A3-414E-BFE7-EA698EB0D1DD}"/>
   <bookViews>
-    <workbookView xWindow="29790" yWindow="480" windowWidth="27300" windowHeight="14160" tabRatio="856" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29790" yWindow="480" windowWidth="27300" windowHeight="14160" tabRatio="856" firstSheet="6" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="11" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="222">
   <si>
     <t>This spreadsheet supports analysis development and production by providing a structured template for documentation</t>
   </si>
@@ -417,7 +417,7 @@
     <t>Do you agree to undertake the roles and responsibilties outlined in the sheet 'R&amp;R Resources'?</t>
   </si>
   <si>
-    <t>Please record here the documents you have created to evidence your work in your role</t>
+    <t>Please link here the documents you have created to evidence your work in your role</t>
   </si>
   <si>
     <t>Date of last review/update</t>
@@ -706,10 +706,10 @@
   </si>
   <si>
     <t>This sheet is a record of past performed quality assurance and future planned quality assurance.
-Each review should be signed off by the Analyitcal Assurer only after
+Each review should be signed off by the Analytical Assurer only after
 a) The review has been performed 
-b) The analysis team have recrived the findings of the review
-c) The analytical assurer is sure that the analysis team have understood the findings of the review and have planned  actions based on the review findings.</t>
+b) The analysis team have received the findings of the review
+c) The Analytical Assurer is sure that the analysis team have understood the findings of the review and have planned actions based on the review findings.</t>
   </si>
   <si>
     <t>QA Round</t>
@@ -816,11 +816,18 @@
   </si>
   <si>
     <t>Assumptions are made whenever data enters the analysis, a process is applied to data, or an interpretation of the data occurs.
+Assumptions might rely on other assumptions! Record this fact by putting the numbers of other assumptions this one depends on in the second column.
 Most analysis will make dozens of assumptions for even small, simple workflows. Assumptions are often implicit - we recommend holding a workshop in the team to surface them.
 A good place to start is the assumption that the input data is representative - this can be risk scored, impact scored and tested against known populations to understand how representative your inputs are</t>
   </si>
   <si>
+    <t>Assumptions might rely on other assumptions! Record this fact by putting the numbers of other assumptions this one depends on in the second column.</t>
+  </si>
+  <si>
     <t>Assumption ID</t>
+  </si>
+  <si>
+    <t>This Assumption depends on other Assumptions:</t>
   </si>
   <si>
     <t>Location in code, documentation or publication</t>
@@ -1005,7 +1012,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1248,7 +1255,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1329,17 +1336,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1360,30 +1356,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1736,28 +1712,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1771,27 +1747,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1800,7 +1776,7 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1813,15 +1789,15 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1843,28 +1819,28 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1908,13 +1884,13 @@
     <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1926,44 +1902,44 @@
     <xf numFmtId="0" fontId="25" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1971,32 +1947,29 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2010,15 +1983,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2028,12 +1992,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2861,11 +2833,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0E718D-ABA6-478B-BFB8-19647D312746}">
   <dimension ref="B2:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="45"/>
     <col min="2" max="2" width="15.7109375" style="80" customWidth="1"/>
@@ -2874,27 +2846,27 @@
     <col min="5" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2" s="99" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4">
       <c r="B3" s="99" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" s="99" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4">
       <c r="B5" s="99" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" s="56" t="s">
         <v>4</v>
       </c>
@@ -2905,7 +2877,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="30">
       <c r="B8" s="56" t="s">
         <v>7</v>
       </c>
@@ -2914,7 +2886,7 @@
       </c>
       <c r="D8" s="79"/>
     </row>
-    <row r="9" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="45">
       <c r="B9" s="56" t="s">
         <v>9</v>
       </c>
@@ -2923,7 +2895,7 @@
       </c>
       <c r="D9" s="79"/>
     </row>
-    <row r="10" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="60">
       <c r="B10" s="56" t="s">
         <v>11</v>
       </c>
@@ -2934,7 +2906,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4">
       <c r="B11" s="56" t="s">
         <v>14</v>
       </c>
@@ -2943,7 +2915,7 @@
       </c>
       <c r="D11" s="79"/>
     </row>
-    <row r="12" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" ht="45">
       <c r="B12" s="56" t="s">
         <v>16</v>
       </c>
@@ -2952,7 +2924,7 @@
       </c>
       <c r="D12" s="79"/>
     </row>
-    <row r="13" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" ht="75">
       <c r="B13" s="54" t="s">
         <v>18</v>
       </c>
@@ -2961,7 +2933,7 @@
       </c>
       <c r="D13" s="81"/>
     </row>
-    <row r="14" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" ht="90">
       <c r="B14" s="56" t="s">
         <v>20</v>
       </c>
@@ -2970,7 +2942,7 @@
       </c>
       <c r="D14" s="79"/>
     </row>
-    <row r="15" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="45">
       <c r="B15" s="56" t="s">
         <v>22</v>
       </c>
@@ -2979,7 +2951,7 @@
       </c>
       <c r="D15" s="79"/>
     </row>
-    <row r="16" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="30">
       <c r="B16" s="56" t="s">
         <v>24</v>
       </c>
@@ -2988,24 +2960,24 @@
       </c>
       <c r="D16" s="79"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4">
       <c r="C17" s="80"/>
       <c r="D17" s="80"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4">
       <c r="C18" s="80"/>
       <c r="D18" s="80"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4">
       <c r="D19" s="52"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4">
       <c r="D20" s="52"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4">
       <c r="D21" s="52"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4">
       <c r="D22" s="52"/>
     </row>
   </sheetData>
@@ -3024,21 +2996,21 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
       <c r="B3" s="88" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3060,7 +3032,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="1"/>
     <col min="2" max="2" width="42.85546875" style="1" customWidth="1"/>
@@ -3070,105 +3042,105 @@
     <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="30">
       <c r="B2" s="25" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="48.95" customHeight="1">
       <c r="B4" s="25" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
       <c r="B5" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
       <c r="D6" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="23.45" customHeight="1">
       <c r="D7" s="34"/>
       <c r="E7" s="35"/>
       <c r="F7" s="35"/>
       <c r="G7" s="35"/>
       <c r="H7" s="36" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="I7" s="35"/>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="2:10" ht="6.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="6.95" customHeight="1">
       <c r="D8" s="37"/>
       <c r="J8" s="26"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="D9" s="38"/>
       <c r="G9" s="29" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H9" s="29" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="J9" s="26"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10">
       <c r="D10" s="38"/>
       <c r="F10" s="28" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="I10" s="33" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="J10" s="26"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10">
       <c r="D11" s="39" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="G11" s="33" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H11" s="33" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="I11" s="33" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="J11" s="26"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10">
       <c r="D12" s="38"/>
       <c r="F12" s="28" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="I12" s="33" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="J12" s="26"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10">
       <c r="D13" s="31"/>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
@@ -3177,14 +3149,14 @@
       <c r="I13" s="27"/>
       <c r="J13" s="30"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10">
       <c r="B15" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
       <c r="B16" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3200,31 +3172,31 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" s="124" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -3240,10 +3212,10 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="A1:D26"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="45"/>
     <col min="2" max="2" width="23.5703125" style="53" customWidth="1"/>
@@ -3252,7 +3224,7 @@
     <col min="5" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="46" t="s">
         <v>26</v>
       </c>
@@ -3260,25 +3232,25 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="B2" s="54" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="49"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="B3" s="55" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="50"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="B4" s="55" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="50"/>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="45">
       <c r="B5" s="55" t="s">
         <v>31</v>
       </c>
@@ -3287,41 +3259,41 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="B6" s="56" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="48"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="46" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="B9" s="54" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="49"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="B10" s="56" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="47"/>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="30">
       <c r="B11" s="57" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="51"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="46" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="60">
       <c r="B14" s="56" t="s">
         <v>39</v>
       </c>
@@ -3330,7 +3302,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="30">
       <c r="B15" s="56" t="s">
         <v>41</v>
       </c>
@@ -3339,7 +3311,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="30">
       <c r="B16" s="56" t="s">
         <v>43</v>
       </c>
@@ -3348,12 +3320,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="46"/>
       <c r="B19" s="54" t="s">
         <v>46</v>
@@ -3363,14 +3335,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="46"/>
       <c r="B20" s="54" t="s">
         <v>48</v>
       </c>
       <c r="C20" s="50"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="B21" s="56" t="s">
         <v>49</v>
       </c>
@@ -3379,25 +3351,25 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" s="46" customFormat="1">
       <c r="A23" s="46" t="s">
         <v>51</v>
       </c>
       <c r="B23" s="53"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="B24" s="56" t="s">
         <v>52</v>
       </c>
       <c r="C24" s="48"/>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="30">
       <c r="B25" s="54" t="s">
         <v>53</v>
       </c>
       <c r="C25" s="50"/>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="30">
       <c r="B26" s="56" t="s">
         <v>54</v>
       </c>
@@ -3423,7 +3395,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="45"/>
     <col min="2" max="2" width="27.140625" style="77" customWidth="1"/>
@@ -3436,10 +3408,10 @@
     <col min="9" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="76"/>
     </row>
-    <row r="2" spans="1:8" s="75" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="75" customFormat="1">
       <c r="A2" s="74"/>
       <c r="B2" s="89" t="s">
         <v>55</v>
@@ -3447,22 +3419,22 @@
       <c r="D2" s="74"/>
       <c r="F2" s="78"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="B3" s="89" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="B4" s="89" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="B5" s="91" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="45" t="s">
         <v>59</v>
       </c>
@@ -3470,7 +3442,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="74" customFormat="1">
       <c r="B8" s="53" t="s">
         <v>61</v>
       </c>
@@ -3484,14 +3456,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="46"/>
       <c r="B10" s="95" t="s">
         <v>65</v>
       </c>
       <c r="F10" s="45"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="B11" s="93" t="s">
         <v>66</v>
       </c>
@@ -3505,7 +3477,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" customHeight="1">
       <c r="B12" s="94" t="s">
         <v>70</v>
       </c>
@@ -3519,21 +3491,21 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="B13" s="91"/>
       <c r="F13" s="45"/>
       <c r="H13" s="96" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="B14" s="91"/>
       <c r="F14" s="45"/>
       <c r="H14" s="96" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="46"/>
       <c r="B15" s="95" t="s">
         <v>76</v>
@@ -3541,34 +3513,34 @@
       <c r="F15" s="45"/>
       <c r="H15" s="96"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="B16" s="93" t="s">
         <v>77</v>
       </c>
       <c r="D16" s="92"/>
       <c r="F16" s="45"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="B17" s="93" t="s">
         <v>78</v>
       </c>
       <c r="D17" s="92"/>
       <c r="F17" s="45"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="B18" s="91"/>
       <c r="D18" s="92"/>
       <c r="F18" s="45"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="B19" s="91"/>
       <c r="F19" s="45"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="B20" s="91"/>
       <c r="F20" s="45"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="45" t="s">
         <v>79</v>
       </c>
@@ -3577,63 +3549,63 @@
       </c>
       <c r="F21" s="45"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="B22" s="91" t="s">
         <v>81</v>
       </c>
       <c r="F22" s="45"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="B23" s="91"/>
       <c r="F23" s="45"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="46"/>
       <c r="B24" s="91"/>
       <c r="F24" s="45"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="46"/>
       <c r="B25" s="91"/>
       <c r="F25" s="45"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="B26" s="91"/>
       <c r="F26" s="45"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="B27" s="91"/>
       <c r="F27" s="45"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="B28" s="91"/>
       <c r="F28" s="45"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="B29" s="91"/>
       <c r="F29" s="45"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="B30" s="91"/>
       <c r="F30" s="45"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="B31" s="91"/>
       <c r="F31" s="45"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="B32" s="91"/>
       <c r="F32" s="45"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6">
       <c r="B33" s="91"/>
       <c r="F33" s="45"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6">
       <c r="B34" s="91"/>
       <c r="F34" s="45"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6">
       <c r="B35" s="91"/>
       <c r="F35" s="45"/>
     </row>
@@ -3650,11 +3622,11 @@
   </sheetPr>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="24.42578125" style="42" customWidth="1"/>
@@ -3668,12 +3640,12 @@
     <col min="11" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
     </row>
-    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="18.75">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
@@ -3688,7 +3660,7 @@
       <c r="J2" s="13"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -3701,7 +3673,7 @@
       <c r="J3" s="13"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75">
       <c r="A4" s="6"/>
       <c r="B4" s="125" t="s">
         <v>83</v>
@@ -3716,7 +3688,7 @@
       <c r="J4" s="13"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75">
       <c r="A5" s="6"/>
       <c r="B5" s="127"/>
       <c r="C5" s="128"/>
@@ -3729,7 +3701,7 @@
       <c r="J5" s="13"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.75">
       <c r="A6" s="6"/>
       <c r="B6" s="127"/>
       <c r="C6" s="128"/>
@@ -3742,7 +3714,7 @@
       <c r="J6" s="13"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75">
       <c r="A7" s="6"/>
       <c r="B7" s="129"/>
       <c r="C7" s="130"/>
@@ -3755,7 +3727,7 @@
       <c r="J7" s="13"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3768,12 +3740,12 @@
       <c r="J8" s="13"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="36">
       <c r="B10" s="8" t="s">
         <v>84</v>
       </c>
@@ -3802,7 +3774,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="17"/>
       <c r="B11" s="43" t="s">
         <v>93</v>
@@ -3817,7 +3789,7 @@
       <c r="J11" s="14"/>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="9"/>
       <c r="B12" s="43" t="s">
         <v>94</v>
@@ -3832,7 +3804,7 @@
       <c r="J12" s="15"/>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="B13" s="44" t="s">
         <v>95</v>
       </c>
@@ -3845,15 +3817,15 @@
       <c r="I13" s="41"/>
       <c r="J13" s="41"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="42" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="B16" s="43" t="s">
         <v>93</v>
       </c>
@@ -3866,7 +3838,7 @@
       <c r="I16" s="15"/>
       <c r="J16" s="14"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10">
       <c r="B17" s="43" t="s">
         <v>94</v>
       </c>
@@ -3879,7 +3851,7 @@
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10">
       <c r="B18" s="44" t="s">
         <v>95</v>
       </c>
@@ -3917,7 +3889,7 @@
       <selection sqref="A1:N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" style="62" customWidth="1"/>
     <col min="2" max="2" width="103.28515625" style="62" customWidth="1"/>
@@ -3933,20 +3905,20 @@
     <col min="14" max="16384" width="9.140625" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15">
       <c r="A1" s="61" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15">
       <c r="A2" s="63" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="61"/>
     </row>
-    <row r="4" spans="1:14" ht="87.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="87.75">
       <c r="A4" s="100" t="s">
         <v>99</v>
       </c>
@@ -3969,13 +3941,13 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="61"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" s="61"/>
     </row>
-    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15">
       <c r="A7" s="72" t="s">
         <v>105</v>
       </c>
@@ -3987,7 +3959,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="65" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="65" customFormat="1" ht="15">
       <c r="B8" s="67" t="s">
         <v>108</v>
       </c>
@@ -4016,7 +3988,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="28.5">
       <c r="B9" s="60" t="s">
         <v>111</v>
       </c>
@@ -4033,7 +4005,7 @@
       <c r="M9" s="69"/>
       <c r="N9" s="69"/>
     </row>
-    <row r="10" spans="1:14" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="42.75">
       <c r="B10" s="60" t="s">
         <v>114</v>
       </c>
@@ -4050,7 +4022,7 @@
       <c r="M10" s="69"/>
       <c r="N10" s="69"/>
     </row>
-    <row r="11" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="28.5">
       <c r="B11" s="60" t="s">
         <v>117</v>
       </c>
@@ -4067,7 +4039,7 @@
       <c r="M11" s="69"/>
       <c r="N11" s="69"/>
     </row>
-    <row r="12" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="28.5">
       <c r="B12" s="60" t="s">
         <v>120</v>
       </c>
@@ -4084,7 +4056,7 @@
       <c r="M12" s="69"/>
       <c r="N12" s="69"/>
     </row>
-    <row r="13" spans="1:14" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="42.75">
       <c r="B13" s="60" t="s">
         <v>123</v>
       </c>
@@ -4101,7 +4073,7 @@
       <c r="M13" s="69"/>
       <c r="N13" s="69"/>
     </row>
-    <row r="14" spans="1:14" ht="44.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="44.25">
       <c r="B14" s="71" t="s">
         <v>126</v>
       </c>
@@ -4116,7 +4088,7 @@
       <c r="M14" s="69"/>
       <c r="N14" s="69"/>
     </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15">
       <c r="A16" s="65" t="s">
         <v>128</v>
       </c>
@@ -4127,7 +4099,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="7:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:14" ht="15">
       <c r="G17" s="68" t="s">
         <v>131</v>
       </c>
@@ -4147,7 +4119,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="7:14" ht="100.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="7:14" ht="100.5">
       <c r="G18" s="106" t="s">
         <v>134</v>
       </c>
@@ -4177,11 +4149,11 @@
   <dimension ref="A2:H36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <pane ySplit="10" topLeftCell="C12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
@@ -4194,7 +4166,7 @@
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" s="6" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="23.25">
       <c r="D2" s="7" t="s">
         <v>137</v>
       </c>
@@ -4203,53 +4175,53 @@
       </c>
       <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="6" customFormat="1" ht="15.75">
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="125" t="s">
+    <row r="4" spans="1:8" s="6" customFormat="1" ht="15.75">
+      <c r="B4" s="144" t="s">
         <v>139</v>
       </c>
-      <c r="C4" s="131"/>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="132"/>
+      <c r="C4" s="144"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="145"/>
+      <c r="F4" s="145"/>
+      <c r="G4" s="145"/>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="127"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="133"/>
+    <row r="5" spans="1:8" s="6" customFormat="1" ht="15.75">
+      <c r="B5" s="145"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="145"/>
       <c r="H5" s="13"/>
     </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="127"/>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="133"/>
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="15.75">
+      <c r="B6" s="145"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="129"/>
-      <c r="C7" s="130"/>
-      <c r="D7" s="130"/>
-      <c r="E7" s="130"/>
-      <c r="F7" s="130"/>
-      <c r="G7" s="134"/>
+    <row r="7" spans="1:8" s="6" customFormat="1" ht="15.75">
+      <c r="B7" s="145"/>
+      <c r="C7" s="145"/>
+      <c r="D7" s="145"/>
+      <c r="E7" s="145"/>
+      <c r="F7" s="145"/>
+      <c r="G7" s="145"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="6" customFormat="1" ht="15.75">
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="B10" s="8" t="s">
         <v>140</v>
       </c>
@@ -4272,7 +4244,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="9" customFormat="1" ht="105" customHeight="1">
       <c r="A11" s="17"/>
       <c r="B11" s="10">
         <v>1</v>
@@ -4294,100 +4266,100 @@
       </c>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="9" customFormat="1">
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="H12" s="19"/>
     </row>
-    <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="9" customFormat="1">
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="H13" s="19"/>
     </row>
-    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="9" customFormat="1">
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="H14" s="19"/>
     </row>
-    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="9" customFormat="1">
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="9" customFormat="1">
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="4:8" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" s="9" customFormat="1">
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" s="9" customFormat="1">
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" s="9" customFormat="1">
       <c r="H20" s="20"/>
     </row>
-    <row r="21" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" s="9" customFormat="1">
       <c r="H21" s="20"/>
     </row>
-    <row r="22" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" s="9" customFormat="1">
       <c r="H22" s="20"/>
     </row>
-    <row r="23" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" s="9" customFormat="1">
       <c r="H23" s="20"/>
     </row>
-    <row r="24" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" s="9" customFormat="1">
       <c r="H24" s="20"/>
     </row>
-    <row r="25" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" s="9" customFormat="1">
       <c r="H25" s="20"/>
     </row>
-    <row r="26" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" s="9" customFormat="1">
       <c r="H26" s="20"/>
     </row>
-    <row r="27" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" s="9" customFormat="1">
       <c r="H27" s="20"/>
     </row>
-    <row r="28" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" s="9" customFormat="1">
       <c r="H28" s="20"/>
     </row>
-    <row r="29" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" s="9" customFormat="1">
       <c r="H29" s="20"/>
     </row>
-    <row r="30" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:8" s="9" customFormat="1">
       <c r="H30" s="20"/>
     </row>
-    <row r="31" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:8" s="9" customFormat="1">
       <c r="H31" s="20"/>
     </row>
-    <row r="32" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:8" s="9" customFormat="1">
       <c r="H32" s="20"/>
     </row>
-    <row r="33" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:8" s="9" customFormat="1">
       <c r="H33" s="20"/>
     </row>
-    <row r="34" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:8" s="9" customFormat="1">
       <c r="H34" s="20"/>
     </row>
-    <row r="35" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:8" s="9" customFormat="1">
       <c r="H35" s="20"/>
     </row>
-    <row r="36" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:8" s="9" customFormat="1">
       <c r="H36" s="20"/>
     </row>
   </sheetData>
@@ -4410,11 +4382,11 @@
   </sheetPr>
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="1"/>
     <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
@@ -4432,12 +4404,12 @@
     <col min="14" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="23.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
@@ -4456,7 +4428,7 @@
       <c r="L2" s="13"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15.75">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -4471,69 +4443,69 @@
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15.75">
       <c r="A4" s="6"/>
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="131" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="136"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="137"/>
+      <c r="C4" s="132"/>
+      <c r="D4" s="132"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="132"/>
+      <c r="H4" s="133"/>
       <c r="I4" s="40"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15.75">
       <c r="A5" s="6"/>
-      <c r="B5" s="138"/>
+      <c r="B5" s="134"/>
       <c r="C5" s="128"/>
       <c r="D5" s="128"/>
       <c r="E5" s="128"/>
       <c r="F5" s="128"/>
       <c r="G5" s="128"/>
-      <c r="H5" s="139"/>
+      <c r="H5" s="135"/>
       <c r="I5" s="40"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15.75">
       <c r="A6" s="6"/>
-      <c r="B6" s="138"/>
+      <c r="B6" s="134"/>
       <c r="C6" s="128"/>
       <c r="D6" s="128"/>
       <c r="E6" s="128"/>
       <c r="F6" s="128"/>
       <c r="G6" s="128"/>
-      <c r="H6" s="139"/>
+      <c r="H6" s="135"/>
       <c r="I6" s="40"/>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.75">
       <c r="A7" s="6"/>
-      <c r="B7" s="140"/>
-      <c r="C7" s="141"/>
-      <c r="D7" s="141"/>
-      <c r="E7" s="141"/>
-      <c r="F7" s="141"/>
-      <c r="G7" s="141"/>
-      <c r="H7" s="142"/>
+      <c r="B7" s="136"/>
+      <c r="C7" s="137"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
+      <c r="G7" s="137"/>
+      <c r="H7" s="138"/>
       <c r="I7" s="40"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15.75">
       <c r="A8" s="6"/>
       <c r="B8" s="16"/>
       <c r="C8" s="6"/>
@@ -4548,12 +4520,12 @@
       <c r="L8" s="13"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="26.25">
       <c r="B10" s="115" t="s">
         <v>154</v>
       </c>
@@ -4591,7 +4563,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="17"/>
       <c r="B11" s="113" t="s">
         <v>162</v>
@@ -4630,7 +4602,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="9"/>
       <c r="B12" s="113" t="s">
         <v>162</v>
@@ -4669,7 +4641,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="B13" s="113" t="s">
         <v>162</v>
       </c>
@@ -4707,7 +4679,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="B14" s="113" t="s">
         <v>162</v>
       </c>
@@ -4745,7 +4717,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="B15" s="113" t="s">
         <v>162</v>
       </c>
@@ -4783,7 +4755,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="B16" s="113" t="s">
         <v>162</v>
       </c>
@@ -4821,7 +4793,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13">
       <c r="B17" s="113" t="s">
         <v>162</v>
       </c>
@@ -4859,7 +4831,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13">
       <c r="B18" s="113" t="s">
         <v>162</v>
       </c>
@@ -4897,7 +4869,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13">
       <c r="B19" s="113" t="s">
         <v>162</v>
       </c>
@@ -4935,7 +4907,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13">
       <c r="B20" s="113" t="s">
         <v>162</v>
       </c>
@@ -4973,7 +4945,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13">
       <c r="B21" s="113" t="s">
         <v>162</v>
       </c>
@@ -5011,7 +4983,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13">
       <c r="B22" s="113" t="s">
         <v>162</v>
       </c>
@@ -5049,7 +5021,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="2:13" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" ht="26.25">
       <c r="B25" s="111" t="s">
         <v>163</v>
       </c>
@@ -5087,7 +5059,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13">
       <c r="B26" s="113" t="s">
         <v>162</v>
       </c>
@@ -5125,7 +5097,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13">
       <c r="B27" s="113" t="s">
         <v>162</v>
       </c>
@@ -5163,7 +5135,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13">
       <c r="B28" s="113" t="s">
         <v>162</v>
       </c>
@@ -5201,7 +5173,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13">
       <c r="B29" s="113" t="s">
         <v>162</v>
       </c>
@@ -5239,7 +5211,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13">
       <c r="B30" s="113" t="s">
         <v>162</v>
       </c>
@@ -5277,7 +5249,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13">
       <c r="B31" s="113" t="s">
         <v>162</v>
       </c>
@@ -5315,7 +5287,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13">
       <c r="B32" s="113" t="s">
         <v>162</v>
       </c>
@@ -5353,7 +5325,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13">
       <c r="B33" s="113" t="s">
         <v>162</v>
       </c>
@@ -5391,7 +5363,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13">
       <c r="B34" s="113" t="s">
         <v>162</v>
       </c>
@@ -5429,7 +5401,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13">
       <c r="B35" s="113" t="s">
         <v>162</v>
       </c>
@@ -5467,7 +5439,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13">
       <c r="B36" s="113" t="s">
         <v>162</v>
       </c>
@@ -5505,7 +5477,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13">
       <c r="B37" s="113" t="s">
         <v>162</v>
       </c>
@@ -5543,7 +5515,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13">
       <c r="B40" s="120"/>
       <c r="C40" s="120"/>
       <c r="D40" s="120"/>
@@ -5557,7 +5529,7 @@
       <c r="L40" s="120"/>
       <c r="M40" s="121"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13">
       <c r="B41" s="122"/>
       <c r="C41" s="122"/>
       <c r="D41" s="122"/>
@@ -5571,7 +5543,7 @@
       <c r="L41" s="122"/>
       <c r="M41" s="122"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13">
       <c r="B42" s="122"/>
       <c r="C42" s="122"/>
       <c r="D42" s="122"/>
@@ -5585,7 +5557,7 @@
       <c r="L42" s="122"/>
       <c r="M42" s="122"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13">
       <c r="B43" s="122"/>
       <c r="C43" s="122"/>
       <c r="D43" s="122"/>
@@ -5599,7 +5571,7 @@
       <c r="L43" s="122"/>
       <c r="M43" s="122"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13">
       <c r="B44" s="122"/>
       <c r="C44" s="122"/>
       <c r="D44" s="122"/>
@@ -5613,7 +5585,7 @@
       <c r="L44" s="122"/>
       <c r="M44" s="122"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:13">
       <c r="B45" s="122"/>
       <c r="C45" s="122"/>
       <c r="D45" s="122"/>
@@ -5627,7 +5599,7 @@
       <c r="L45" s="122"/>
       <c r="M45" s="122"/>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13">
       <c r="B46" s="122"/>
       <c r="C46" s="122"/>
       <c r="D46" s="122"/>
@@ -5641,7 +5613,7 @@
       <c r="L46" s="122"/>
       <c r="M46" s="122"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13">
       <c r="B47" s="122"/>
       <c r="C47" s="122"/>
       <c r="D47" s="122"/>
@@ -5655,7 +5627,7 @@
       <c r="L47" s="122"/>
       <c r="M47" s="122"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13">
       <c r="B48" s="122"/>
       <c r="C48" s="122"/>
       <c r="D48" s="122"/>
@@ -5669,7 +5641,7 @@
       <c r="L48" s="122"/>
       <c r="M48" s="122"/>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:13">
       <c r="B49" s="122"/>
       <c r="C49" s="122"/>
       <c r="D49" s="122"/>
@@ -5683,7 +5655,7 @@
       <c r="L49" s="122"/>
       <c r="M49" s="122"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:13">
       <c r="B50" s="122"/>
       <c r="C50" s="122"/>
       <c r="D50" s="122"/>
@@ -5697,7 +5669,7 @@
       <c r="L50" s="122"/>
       <c r="M50" s="122"/>
     </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:13">
       <c r="B51" s="122"/>
       <c r="C51" s="122"/>
       <c r="D51" s="122"/>
@@ -5711,7 +5683,7 @@
       <c r="L51" s="122"/>
       <c r="M51" s="122"/>
     </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:13">
       <c r="B52" s="122"/>
       <c r="C52" s="122"/>
       <c r="D52" s="122"/>
@@ -5760,14 +5732,14 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:S36"/>
+  <dimension ref="A2:T36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
@@ -5788,7 +5760,7 @@
     <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" s="6" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" s="6" customFormat="1" ht="23.25">
       <c r="D2" s="7" t="s">
         <v>172</v>
       </c>
@@ -5802,7 +5774,7 @@
       <c r="O2" s="13"/>
       <c r="P2" s="13"/>
     </row>
-    <row r="3" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" s="6" customFormat="1" ht="15.75">
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
@@ -5810,18 +5782,18 @@
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
     </row>
-    <row r="4" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="125" t="s">
+    <row r="4" spans="1:20" s="6" customFormat="1" ht="15.75">
+      <c r="B4" s="144" t="s">
         <v>173</v>
       </c>
-      <c r="C4" s="131"/>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
-      <c r="H4" s="126"/>
-      <c r="I4" s="126"/>
-      <c r="J4" s="132"/>
+      <c r="C4" s="144"/>
+      <c r="D4" s="145"/>
+      <c r="E4" s="145"/>
+      <c r="F4" s="145"/>
+      <c r="G4" s="145"/>
+      <c r="H4" s="145"/>
+      <c r="I4" s="145"/>
+      <c r="J4" s="145"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
@@ -5829,16 +5801,16 @@
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
     </row>
-    <row r="5" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="127"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="128"/>
-      <c r="I5" s="128"/>
-      <c r="J5" s="133"/>
+    <row r="5" spans="1:20" s="6" customFormat="1" ht="15.75">
+      <c r="B5" s="145"/>
+      <c r="C5" s="145"/>
+      <c r="D5" s="145"/>
+      <c r="E5" s="145"/>
+      <c r="F5" s="145"/>
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="145"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
@@ -5846,16 +5818,16 @@
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
     </row>
-    <row r="6" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="127"/>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="133"/>
+    <row r="6" spans="1:20" s="6" customFormat="1" ht="15.75">
+      <c r="B6" s="145"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="145"/>
+      <c r="I6" s="145"/>
+      <c r="J6" s="145"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
@@ -5863,16 +5835,16 @@
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
     </row>
-    <row r="7" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="129"/>
-      <c r="C7" s="130"/>
-      <c r="D7" s="130"/>
-      <c r="E7" s="130"/>
-      <c r="F7" s="130"/>
-      <c r="G7" s="130"/>
-      <c r="H7" s="130"/>
-      <c r="I7" s="130"/>
-      <c r="J7" s="134"/>
+    <row r="7" spans="1:20" s="6" customFormat="1" ht="15.75">
+      <c r="B7" s="145"/>
+      <c r="C7" s="145"/>
+      <c r="D7" s="145"/>
+      <c r="E7" s="145"/>
+      <c r="F7" s="145"/>
+      <c r="G7" s="145"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="145"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
@@ -5880,9 +5852,18 @@
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
-    <row r="8" spans="1:19" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
+    <row r="8" spans="1:20" s="6" customFormat="1" ht="15.75">
+      <c r="B8" s="146" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="147"/>
+      <c r="D8" s="146"/>
+      <c r="E8" s="146"/>
+      <c r="F8" s="146"/>
+      <c r="G8" s="146"/>
+      <c r="H8" s="146"/>
+      <c r="I8" s="146"/>
+      <c r="J8" s="146"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
@@ -5890,92 +5871,96 @@
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
     </row>
-    <row r="10" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="36">
       <c r="B10" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K10" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="L10" s="8" t="s">
-        <v>183</v>
-      </c>
       <c r="M10" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="N10" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="8" t="s">
-        <v>184</v>
-      </c>
       <c r="O10" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="P10" s="84" t="s">
+        <v>186</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q10" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="Q10" s="86" t="s">
-        <v>186</v>
-      </c>
       <c r="R10" s="86" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="S10" s="86" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" s="9" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="T10" s="86" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" s="9" customFormat="1" ht="105" customHeight="1">
       <c r="A11" s="17"/>
       <c r="B11" s="15">
         <v>1</v>
       </c>
       <c r="C11" s="15"/>
-      <c r="D11" s="82"/>
+      <c r="D11" s="15"/>
       <c r="E11" s="82"/>
       <c r="F11" s="82"/>
       <c r="G11" s="82"/>
       <c r="H11" s="82"/>
       <c r="I11" s="82"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="14"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="119"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="15"/>
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
-      <c r="Q11" s="85" t="s">
-        <v>189</v>
-      </c>
-      <c r="R11" s="87" t="s">
-        <v>190</v>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="85" t="s">
+        <v>191</v>
       </c>
       <c r="S11" s="87" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+      <c r="T11" s="87" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="9" customFormat="1">
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
@@ -5990,7 +5975,7 @@
       <c r="P12" s="20"/>
       <c r="Q12" s="22"/>
     </row>
-    <row r="13" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" s="9" customFormat="1">
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
@@ -6005,7 +5990,7 @@
       <c r="P13" s="20"/>
       <c r="Q13" s="22"/>
     </row>
-    <row r="14" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" s="9" customFormat="1">
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
@@ -6020,7 +6005,7 @@
       <c r="P14" s="20"/>
       <c r="Q14" s="21"/>
     </row>
-    <row r="15" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" s="9" customFormat="1">
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
@@ -6035,7 +6020,7 @@
       <c r="P15" s="20"/>
       <c r="Q15" s="21"/>
     </row>
-    <row r="16" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" s="9" customFormat="1">
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
@@ -6050,7 +6035,7 @@
       <c r="P16" s="20"/>
       <c r="Q16" s="21"/>
     </row>
-    <row r="17" spans="4:17" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:17" s="9" customFormat="1" ht="14.25" customHeight="1">
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
@@ -6065,7 +6050,7 @@
       <c r="P17" s="20"/>
       <c r="Q17" s="21"/>
     </row>
-    <row r="18" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:17" s="9" customFormat="1">
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
@@ -6080,7 +6065,7 @@
       <c r="P18" s="20"/>
       <c r="Q18" s="21"/>
     </row>
-    <row r="19" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:17" s="9" customFormat="1">
       <c r="K19" s="20"/>
       <c r="L19" s="20"/>
       <c r="M19" s="20"/>
@@ -6089,7 +6074,7 @@
       <c r="P19" s="20"/>
       <c r="Q19" s="22"/>
     </row>
-    <row r="20" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:17" s="9" customFormat="1">
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -6098,7 +6083,7 @@
       <c r="P20" s="20"/>
       <c r="Q20" s="22"/>
     </row>
-    <row r="21" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:17" s="9" customFormat="1">
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
@@ -6107,7 +6092,7 @@
       <c r="P21" s="20"/>
       <c r="Q21" s="22"/>
     </row>
-    <row r="22" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:17" s="9" customFormat="1">
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
@@ -6116,7 +6101,7 @@
       <c r="P22" s="20"/>
       <c r="Q22" s="22"/>
     </row>
-    <row r="23" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:17" s="9" customFormat="1">
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
       <c r="M23" s="20"/>
@@ -6125,7 +6110,7 @@
       <c r="P23" s="20"/>
       <c r="Q23" s="22"/>
     </row>
-    <row r="24" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:17" s="9" customFormat="1">
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
@@ -6134,7 +6119,7 @@
       <c r="P24" s="20"/>
       <c r="Q24" s="22"/>
     </row>
-    <row r="25" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:17" s="9" customFormat="1">
       <c r="K25" s="20"/>
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
@@ -6143,7 +6128,7 @@
       <c r="P25" s="20"/>
       <c r="Q25" s="22"/>
     </row>
-    <row r="26" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:17" s="9" customFormat="1">
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
@@ -6152,7 +6137,7 @@
       <c r="P26" s="20"/>
       <c r="Q26" s="22"/>
     </row>
-    <row r="27" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:17" s="9" customFormat="1">
       <c r="K27" s="20"/>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
@@ -6161,7 +6146,7 @@
       <c r="P27" s="20"/>
       <c r="Q27" s="22"/>
     </row>
-    <row r="28" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:17" s="9" customFormat="1">
       <c r="K28" s="20"/>
       <c r="L28" s="20"/>
       <c r="M28" s="20"/>
@@ -6170,7 +6155,7 @@
       <c r="P28" s="20"/>
       <c r="Q28" s="22"/>
     </row>
-    <row r="29" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:17" s="9" customFormat="1">
       <c r="K29" s="20"/>
       <c r="L29" s="20"/>
       <c r="M29" s="20"/>
@@ -6179,7 +6164,7 @@
       <c r="P29" s="20"/>
       <c r="Q29" s="22"/>
     </row>
-    <row r="30" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:17" s="9" customFormat="1">
       <c r="K30" s="20"/>
       <c r="L30" s="20"/>
       <c r="M30" s="20"/>
@@ -6188,7 +6173,7 @@
       <c r="P30" s="20"/>
       <c r="Q30" s="22"/>
     </row>
-    <row r="31" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:17" s="9" customFormat="1">
       <c r="K31" s="20"/>
       <c r="L31" s="20"/>
       <c r="M31" s="20"/>
@@ -6197,7 +6182,7 @@
       <c r="P31" s="20"/>
       <c r="Q31" s="22"/>
     </row>
-    <row r="32" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:17" s="9" customFormat="1">
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
       <c r="M32" s="20"/>
@@ -6206,7 +6191,7 @@
       <c r="P32" s="20"/>
       <c r="Q32" s="22"/>
     </row>
-    <row r="33" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:17" s="9" customFormat="1">
       <c r="K33" s="20"/>
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
@@ -6215,7 +6200,7 @@
       <c r="P33" s="20"/>
       <c r="Q33" s="22"/>
     </row>
-    <row r="34" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:17" s="9" customFormat="1">
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
       <c r="M34" s="20"/>
@@ -6224,7 +6209,7 @@
       <c r="P34" s="20"/>
       <c r="Q34" s="22"/>
     </row>
-    <row r="35" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:17" s="9" customFormat="1">
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
       <c r="M35" s="20"/>
@@ -6233,7 +6218,7 @@
       <c r="P35" s="20"/>
       <c r="Q35" s="22"/>
     </row>
-    <row r="36" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="11:17" s="9" customFormat="1">
       <c r="K36" s="20"/>
       <c r="L36" s="20"/>
       <c r="M36" s="20"/>
@@ -6246,7 +6231,7 @@
   <mergeCells count="1">
     <mergeCell ref="B4:J7"/>
   </mergeCells>
-  <conditionalFormatting sqref="Q11:Q36">
+  <conditionalFormatting sqref="Q12:Q36 R11">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
@@ -6258,7 +6243,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q11:Q36" xr:uid="{4E9472C3-0F59-436D-B36A-0DE15C8EE443}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q12:Q36 R11" xr:uid="{4E9472C3-0F59-436D-B36A-0DE15C8EE443}">
       <formula1>"Red, Amber, Green"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6282,7 +6267,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="30" style="1" customWidth="1"/>
@@ -6295,81 +6280,81 @@
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="138.75" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="139" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="109" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F2" s="142" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="H2" s="83" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="144.75" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="143"/>
+      <c r="G3" s="110" t="s">
+        <v>200</v>
+      </c>
+      <c r="H3" s="83" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="121.5" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="107" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F4" s="143"/>
+      <c r="G4" s="110" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="109" t="s">
-        <v>189</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="F2" s="146" t="s">
-        <v>194</v>
-      </c>
-      <c r="G2" s="110" t="s">
-        <v>191</v>
-      </c>
-      <c r="H2" s="83" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="144"/>
-      <c r="C3" s="108" t="s">
-        <v>196</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="147"/>
-      <c r="G3" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="H3" s="83" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="145"/>
-      <c r="C4" s="107" t="s">
-        <v>200</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="F4" s="147"/>
-      <c r="G4" s="110" t="s">
-        <v>190</v>
-      </c>
       <c r="H4" s="83" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="3"/>
       <c r="F7" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="3"/>
     </row>
   </sheetData>
@@ -6397,6 +6382,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031C6D98A8BA9914F9CBD1D8D43561C2B" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20dc68b959a60313fbcac393e99fd10f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e1cd103-0302-4a32-9a4b-e115c950d959" xmlns:ns3="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7195712bd1d9adc40779bc7b93adecf4" ns2:_="" ns3:_="">
     <xsd:import namespace="7e1cd103-0302-4a32-9a4b-e115c950d959"/>
@@ -6639,55 +6633,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71C399E-D560-405D-A693-6A86DF1C82D7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="7e1cd103-0302-4a32-9a4b-e115c950d959"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71C399E-D560-405D-A693-6A86DF1C82D7}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8A29AC-6BF1-4D4D-9282-8A0E51881B4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7e1cd103-0302-4a32-9a4b-e115c950d959"/>
-    <ds:schemaRef ds:uri="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D186559C-C381-484C-9B7A-F4466E79AE25}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D186559C-C381-484C-9B7A-F4466E79AE25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8A29AC-6BF1-4D4D-9282-8A0E51881B4F}"/>
 </file>
</xml_diff>

<commit_message>
Updated README.md to add comprehensive file list
</commit_message>
<xml_diff>
--- a/docs/assumptions_and_decision_log_template.xlsx
+++ b/docs/assumptions_and_decision_log_template.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1010" documentId="8_{C66C9284-12B1-4C2F-AAEC-29ECF8510037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21B1B33D-F6A3-414E-BFE7-EA698EB0D1DD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEFE303-931A-4000-85A8-D26CE28FF02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29790" yWindow="480" windowWidth="27300" windowHeight="14160" tabRatio="856" firstSheet="6" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="26850" windowHeight="14310" tabRatio="856" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="11" r:id="rId1"/>
@@ -103,9 +103,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="222">
   <si>
-    <t>This spreadsheet supports analysis development and production by providing a structured template for documentation</t>
-  </si>
-  <si>
     <t>While most of the template should be self explanatory, this introductory slide sets out basic guidance on use.</t>
   </si>
   <si>
@@ -127,21 +124,12 @@
     <t>Analysis Overview</t>
   </si>
   <si>
-    <t>A table with a series of boxes to be filled in by the owning team which sets out basic details about the analysis</t>
-  </si>
-  <si>
     <t>Analysis Map</t>
   </si>
   <si>
-    <t>A graphical representation of all the inputs into the analysis, what processes they go through and the outputs created by the analysis. These outputs should then, ideally, be linked to planned or ongoing publications.</t>
-  </si>
-  <si>
     <t>Roles &amp; Responsibilities</t>
   </si>
   <si>
-    <t>Records when somebody took on a governance role and if they reviewed the documentation relevant to the responsibiltiies of the role. Also records past governance ownership to ensure that handovers are recorded.</t>
-  </si>
-  <si>
     <t>Guidance about what each assurance role involves and templates to record agreement to carry out that role are on the sheet labelled 'R&amp;R Resources'</t>
   </si>
   <si>
@@ -160,19 +148,10 @@
     <t>Decisions &amp; Issues Register</t>
   </si>
   <si>
-    <t>As issues arise in development, decisions will have to be made about them. Issues can come from QA, or be raised from within the team or by stakeholders. For example, there may be concerns about the validity of one of the inputs used. This requires a decision by the individuals in senior governance positions, who will explain the evidence underpinning this decision. Often these decisions will become assumptions, which are stored in the assumptions log.</t>
-  </si>
-  <si>
     <t>Assumptions Log</t>
   </si>
   <si>
-    <t>This table records the assumptions made about the analysis. Assumptions will often be decisions made because there is a need to simplify the real world so it can be analysed or modelled. Wherever possible, such assumptions should have a numerical value and an uncertainty range around the value. You should also give your assumptions a quality RAG rating. When this is combined with an assessment about how sensitive the analysis is to the assumption, you get an indicative risk score. Use the risk score to inform how resources are allocated to further research and improvement of the assumptions.</t>
-  </si>
-  <si>
     <t>Quality &amp; Sensitivity Guide</t>
-  </si>
-  <si>
-    <t>A at-a-glance guide to quality scoring. If you are not sure about the quality or sensitivity score of an assumption, err on the side of caution and go for lower quality and higher sensitivity.</t>
   </si>
   <si>
     <t>Risk Scoring Guide</t>
@@ -1007,12 +986,34 @@
   <si>
     <t>Resolved</t>
   </si>
+  <si>
+    <t>This spreadsheet supports analysis development and production by providing a structured template for documentation.</t>
+  </si>
+  <si>
+    <t>A table to be filled in by the owning team which sets out basic details about the analysis</t>
+  </si>
+  <si>
+    <t>A graphical representation of all the inputs into the analysis, what processes they go through and the outputs created by the analysis. These outputs should ideally be linked to planned or ongoing publications.</t>
+  </si>
+  <si>
+    <t>Use this tab to record when somebody took on a governance role and if they reviewed the documentation relevant to the responsibiltiies of the role.
+The template also records past governance ownership to ensure that handovers are recorded.</t>
+  </si>
+  <si>
+    <t>As issues arise in development, decisions will be made about them. Issues can come from QA, or be raised from within the team or by stakeholders. For example, there may be concerns about the validity of one of the inputs used. This requires a decision by the individuals in senior governance positions, who will explain the evidence underpinning this decision. Often these decisions will become assumptions, which are stored in the assumptions log.</t>
+  </si>
+  <si>
+    <t>This table records the assumptions made about the analysis. Assumptions will often be decisions made because there is a need to simplify the real world so it can be analysed or modelled. Wherever possible,  assumptions should have a numerical value and an uncertainty range around the value. You should also give your assumptions a quality RAG rating. When this is combined with an assessment about how sensitive the analysis is to the assumption, you get an indicative risk score. Use the risk score to inform how resources are allocated to further research and improvement of the assumptions.</t>
+  </si>
+  <si>
+    <t>An at-a-glance guide to quality scoring. If you are not sure about the quality or sensitivity score of an assumption, err on the side of caution and go for lower quality and higher sensitivity.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1941,6 +1942,8 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1959,6 +1962,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1998,14 +2007,6 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2833,11 +2834,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0E718D-ABA6-478B-BFB8-19647D312746}">
   <dimension ref="B2:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="45"/>
     <col min="2" max="2" width="15.7109375" style="80" customWidth="1"/>
@@ -2846,138 +2847,138 @@
     <col min="5" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="99" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="99" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
-      <c r="B3" s="99" t="s">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="99" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="99" t="s">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="99" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="99" t="s">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="56" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="56" t="s">
+      <c r="C7" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="D7" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="56" t="s">
+    </row>
+    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="56" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="30">
-      <c r="B8" s="56" t="s">
+      <c r="C8" s="79" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8" s="79"/>
+    </row>
+    <row r="9" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C9" s="79" t="s">
+        <v>217</v>
+      </c>
+      <c r="D9" s="79"/>
+    </row>
+    <row r="10" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B10" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="79"/>
-    </row>
-    <row r="9" spans="2:4" ht="45">
-      <c r="B9" s="56" t="s">
+      <c r="C10" s="79" t="s">
+        <v>218</v>
+      </c>
+      <c r="D10" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="79" t="s">
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="79"/>
-    </row>
-    <row r="10" spans="2:4" ht="60">
-      <c r="B10" s="56" t="s">
+      <c r="C11" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="79" t="s">
+      <c r="D11" s="79"/>
+    </row>
+    <row r="12" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="79" t="s">
+      <c r="C12" s="79" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="56" t="s">
+      <c r="D12" s="79"/>
+    </row>
+    <row r="13" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B13" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="C13" s="117" t="s">
+        <v>219</v>
+      </c>
+      <c r="D13" s="81"/>
+    </row>
+    <row r="14" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="B14" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="79"/>
-    </row>
-    <row r="12" spans="2:4" ht="45">
-      <c r="B12" s="56" t="s">
+      <c r="C14" s="118" t="s">
+        <v>220</v>
+      </c>
+      <c r="D14" s="79"/>
+    </row>
+    <row r="15" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="79" t="s">
+      <c r="C15" s="79" t="s">
+        <v>221</v>
+      </c>
+      <c r="D15" s="79"/>
+    </row>
+    <row r="16" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="79"/>
-    </row>
-    <row r="13" spans="2:4" ht="75">
-      <c r="B13" s="54" t="s">
+      <c r="C16" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="117" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="81"/>
-    </row>
-    <row r="14" spans="2:4" ht="90">
-      <c r="B14" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="118" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="79"/>
-    </row>
-    <row r="15" spans="2:4" ht="45">
-      <c r="B15" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="79" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="79"/>
-    </row>
-    <row r="16" spans="2:4" ht="30">
-      <c r="B16" s="56" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="79" t="s">
-        <v>25</v>
-      </c>
       <c r="D16" s="79"/>
     </row>
-    <row r="17" spans="3:4">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="80"/>
       <c r="D17" s="80"/>
     </row>
-    <row r="18" spans="3:4">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" s="80"/>
       <c r="D18" s="80"/>
     </row>
-    <row r="19" spans="3:4">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D19" s="52"/>
     </row>
-    <row r="20" spans="3:4">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D20" s="52"/>
     </row>
-    <row r="21" spans="3:4">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D21" s="52"/>
     </row>
-    <row r="22" spans="3:4">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D22" s="52"/>
     </row>
   </sheetData>
@@ -2996,21 +2997,21 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="88" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -3032,7 +3033,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="1"/>
     <col min="2" max="2" width="42.85546875" style="1" customWidth="1"/>
@@ -3042,105 +3043,105 @@
     <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="30">
+    <row r="2" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="48.95" customHeight="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="23.45" customHeight="1">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="34"/>
       <c r="E7" s="35"/>
       <c r="F7" s="35"/>
       <c r="G7" s="35"/>
       <c r="H7" s="36" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="I7" s="35"/>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="2:10" ht="6.95" customHeight="1">
+    <row r="8" spans="2:10" ht="6.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="37"/>
       <c r="J8" s="26"/>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D9" s="38"/>
       <c r="G9" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="H9" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="H9" s="29" t="s">
-        <v>198</v>
-      </c>
       <c r="I9" s="29" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="J9" s="26"/>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D10" s="38"/>
       <c r="F10" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="H10" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="I10" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="39" t="s">
+        <v>207</v>
+      </c>
+      <c r="F11" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="G10" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="H10" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="I10" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="J10" s="26"/>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="D11" s="39" t="s">
-        <v>214</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>200</v>
-      </c>
       <c r="G11" s="33" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="H11" s="33" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="I11" s="33" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="J11" s="26"/>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D12" s="38"/>
       <c r="F12" s="28" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="I12" s="33" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="J12" s="26"/>
     </row>
-    <row r="13" spans="2:10">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D13" s="31"/>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
@@ -3149,14 +3150,14 @@
       <c r="I13" s="27"/>
       <c r="J13" s="30"/>
     </row>
-    <row r="15" spans="2:10">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -3172,31 +3173,31 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="124" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3211,11 +3212,11 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="45"/>
     <col min="2" max="2" width="23.5703125" style="53" customWidth="1"/>
@@ -3224,154 +3225,154 @@
     <col min="5" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="54" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C2" s="49"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="55" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C3" s="50"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="55" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C4" s="50"/>
     </row>
-    <row r="5" spans="1:4" ht="45">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="55" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C5" s="50"/>
       <c r="D5" s="52" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="48"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="49"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="47"/>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="51"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="46" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B14" s="56" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="B6" s="56" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="48"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="46" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="49"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="B10" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="47"/>
-    </row>
-    <row r="11" spans="1:4" ht="30">
-      <c r="B11" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="51"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="46" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="60">
-      <c r="B14" s="56" t="s">
-        <v>39</v>
       </c>
       <c r="C14" s="48"/>
       <c r="D14" s="58" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="56" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C15" s="48"/>
       <c r="D15" s="58" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="56" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C16" s="48"/>
       <c r="D16" s="58" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="46"/>
       <c r="B19" s="54" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C19" s="50"/>
       <c r="D19" s="98" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="46"/>
       <c r="B20" s="54" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C20" s="50"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="56" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C21" s="48"/>
       <c r="D21" s="98" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="46" customFormat="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="46" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B23" s="53"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="56" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C24" s="48"/>
     </row>
-    <row r="25" spans="1:4" ht="30">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="54" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C25" s="50"/>
     </row>
-    <row r="26" spans="1:4" ht="30">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="56" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C26" s="48"/>
     </row>
@@ -3395,7 +3396,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="45"/>
     <col min="2" max="2" width="27.140625" style="77" customWidth="1"/>
@@ -3408,204 +3409,204 @@
     <col min="9" max="16384" width="9.140625" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="76"/>
     </row>
-    <row r="2" spans="1:8" s="75" customFormat="1">
+    <row r="2" spans="1:8" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="74"/>
       <c r="B2" s="89" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D2" s="74"/>
       <c r="F2" s="78"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="89" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="89" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="91" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="74" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="74" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="90" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="B4" s="89" t="s">
+      <c r="H8" s="74" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="B5" s="91" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="45" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="74" customFormat="1">
-      <c r="B8" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="74" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="90" t="s">
-        <v>63</v>
-      </c>
-      <c r="H8" s="74" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="46"/>
       <c r="B10" s="95" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="45"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="93" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="97" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="94" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="45"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="B11" s="93" t="s">
+      <c r="H12" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="97" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1">
-      <c r="B12" s="94" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="H12" s="96" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="91"/>
       <c r="F13" s="45"/>
       <c r="H13" s="96" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="91"/>
       <c r="F14" s="45"/>
       <c r="H14" s="96" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="46"/>
       <c r="B15" s="95" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F15" s="45"/>
       <c r="H15" s="96"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="93" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D16" s="92"/>
       <c r="F16" s="45"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="93" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D17" s="92"/>
       <c r="F17" s="45"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="91"/>
       <c r="D18" s="92"/>
       <c r="F18" s="45"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="91"/>
       <c r="F19" s="45"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="91"/>
       <c r="F20" s="45"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B21" s="91" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F21" s="45"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="91" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F22" s="45"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="91"/>
       <c r="F23" s="45"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="46"/>
       <c r="B24" s="91"/>
       <c r="F24" s="45"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
       <c r="B25" s="91"/>
       <c r="F25" s="45"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="91"/>
       <c r="F26" s="45"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="91"/>
       <c r="F27" s="45"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="91"/>
       <c r="F28" s="45"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="91"/>
       <c r="F29" s="45"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="91"/>
       <c r="F30" s="45"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="91"/>
       <c r="F31" s="45"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="91"/>
       <c r="F32" s="45"/>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="91"/>
       <c r="F33" s="45"/>
     </row>
-    <row r="34" spans="2:6">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="91"/>
       <c r="F34" s="45"/>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="91"/>
       <c r="F35" s="45"/>
     </row>
@@ -3622,11 +3623,11 @@
   </sheetPr>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="24.42578125" style="42" customWidth="1"/>
@@ -3640,16 +3641,16 @@
     <col min="11" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
     </row>
-    <row r="2" spans="1:11" ht="18.75">
+    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="6"/>
@@ -3660,7 +3661,7 @@
       <c r="J2" s="13"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -3673,61 +3674,61 @@
       <c r="J3" s="13"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75">
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="B4" s="125" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="126"/>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
+      <c r="B4" s="127" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="128"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75">
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="127"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
+      <c r="B5" s="129"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75">
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="127"/>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
+      <c r="B6" s="129"/>
+      <c r="C6" s="130"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75">
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="129"/>
-      <c r="C7" s="130"/>
-      <c r="D7" s="130"/>
-      <c r="E7" s="130"/>
-      <c r="F7" s="130"/>
-      <c r="G7" s="130"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="132"/>
+      <c r="D7" s="132"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="132"/>
+      <c r="G7" s="132"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75">
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3740,44 +3741,44 @@
       <c r="J8" s="13"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:11" ht="36">
+    <row r="10" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="43" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -3789,10 +3790,10 @@
       <c r="J11" s="14"/>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="43" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -3804,9 +3805,9 @@
       <c r="J12" s="15"/>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="44" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
@@ -3817,17 +3818,17 @@
       <c r="I13" s="41"/>
       <c r="J13" s="41"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G14" s="18"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="43" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -3838,9 +3839,9 @@
       <c r="I16" s="15"/>
       <c r="J16" s="14"/>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="43" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -3851,9 +3852,9 @@
       <c r="I17" s="15"/>
       <c r="J17" s="15"/>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="44" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C18" s="41"/>
       <c r="D18" s="41"/>
@@ -3889,7 +3890,7 @@
       <selection sqref="A1:N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.85546875" style="62" customWidth="1"/>
     <col min="2" max="2" width="103.28515625" style="62" customWidth="1"/>
@@ -3905,182 +3906,182 @@
     <col min="14" max="16384" width="9.140625" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15">
+    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="61"/>
     </row>
-    <row r="4" spans="1:14" ht="87.75">
+    <row r="4" spans="1:14" ht="87.75" x14ac:dyDescent="0.2">
       <c r="A4" s="100" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B4" s="102" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F4" s="101" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G4" s="103" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H4" s="73"/>
       <c r="I4" s="73"/>
       <c r="J4" s="73"/>
       <c r="K4" s="64" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="L4" s="103" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="61"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="61"/>
     </row>
-    <row r="7" spans="1:14" ht="15">
+    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="72" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F7" s="72" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G7" s="66"/>
       <c r="K7" s="65" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" s="65" customFormat="1" ht="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="65" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="67" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C8" s="67" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D8" s="67" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="G8" s="67" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="H8" s="67" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="I8" s="67" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="L8" s="67" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="M8" s="67" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="N8" s="67" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="28.5">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B9" s="60" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C9" s="69"/>
       <c r="D9" s="69"/>
       <c r="G9" s="104" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H9" s="69"/>
       <c r="I9" s="69"/>
       <c r="L9" s="104" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="M9" s="69"/>
       <c r="N9" s="69"/>
     </row>
-    <row r="10" spans="1:14" ht="42.75">
+    <row r="10" spans="1:14" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B10" s="60" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C10" s="69"/>
       <c r="D10" s="69"/>
       <c r="G10" s="70" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="H10" s="69"/>
       <c r="I10" s="69"/>
       <c r="L10" s="104" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="M10" s="69"/>
       <c r="N10" s="69"/>
     </row>
-    <row r="11" spans="1:14" ht="28.5">
+    <row r="11" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B11" s="60" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C11" s="69"/>
       <c r="D11" s="69"/>
       <c r="G11" s="104" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="H11" s="69"/>
       <c r="I11" s="69"/>
       <c r="L11" s="70" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="M11" s="69"/>
       <c r="N11" s="69"/>
     </row>
-    <row r="12" spans="1:14" ht="28.5">
+    <row r="12" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B12" s="60" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C12" s="69"/>
       <c r="D12" s="69"/>
       <c r="G12" s="104" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="H12" s="69"/>
       <c r="I12" s="69"/>
       <c r="L12" s="104" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="M12" s="69"/>
       <c r="N12" s="69"/>
     </row>
-    <row r="13" spans="1:14" ht="42.75">
+    <row r="13" spans="1:14" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B13" s="60" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C13" s="69"/>
       <c r="D13" s="69"/>
       <c r="G13" s="105" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="H13" s="69"/>
       <c r="I13" s="69"/>
       <c r="L13" s="60" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="M13" s="69"/>
       <c r="N13" s="69"/>
     </row>
-    <row r="14" spans="1:14" ht="44.25">
+    <row r="14" spans="1:14" ht="44.25" x14ac:dyDescent="0.25">
       <c r="B14" s="71" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C14" s="69"/>
       <c r="D14" s="69"/>
       <c r="G14" s="105" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H14" s="69"/>
       <c r="I14" s="69"/>
@@ -4088,48 +4089,48 @@
       <c r="M14" s="69"/>
       <c r="N14" s="69"/>
     </row>
-    <row r="16" spans="1:14" ht="15">
+    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="65" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F16" s="65" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="K16" s="65" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="7:14" ht="15">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="7:14" ht="15" x14ac:dyDescent="0.25">
       <c r="G17" s="68" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H17" s="67" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="I17" s="67" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="L17" s="67" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="M17" s="67" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="N17" s="67" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="7:14" ht="100.5">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="7:14" ht="100.5" x14ac:dyDescent="0.2">
       <c r="G18" s="106" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="H18" s="69"/>
       <c r="I18" s="69"/>
       <c r="J18" s="62" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="L18" s="106" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="M18" s="69"/>
       <c r="N18" s="69"/>
@@ -4149,11 +4150,11 @@
   <dimension ref="A2:H36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="C12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="10" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
@@ -4166,200 +4167,200 @@
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" s="6" customFormat="1" ht="23.25">
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="D2" s="7" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="1:8" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="1:8" s="6" customFormat="1" ht="15.75">
-      <c r="B4" s="144" t="s">
-        <v>139</v>
-      </c>
-      <c r="C4" s="144"/>
-      <c r="D4" s="145"/>
-      <c r="E4" s="145"/>
-      <c r="F4" s="145"/>
-      <c r="G4" s="145"/>
+    <row r="4" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="133" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="133"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="134"/>
+      <c r="F4" s="134"/>
+      <c r="G4" s="134"/>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" ht="15.75">
-      <c r="B5" s="145"/>
-      <c r="C5" s="145"/>
-      <c r="D5" s="145"/>
-      <c r="E5" s="145"/>
-      <c r="F5" s="145"/>
-      <c r="G5" s="145"/>
+    <row r="5" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="134"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
       <c r="H5" s="13"/>
     </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" ht="15.75">
-      <c r="B6" s="145"/>
-      <c r="C6" s="145"/>
-      <c r="D6" s="145"/>
-      <c r="E6" s="145"/>
-      <c r="F6" s="145"/>
-      <c r="G6" s="145"/>
+    <row r="6" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="134"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" ht="15.75">
-      <c r="B7" s="145"/>
-      <c r="C7" s="145"/>
-      <c r="D7" s="145"/>
-      <c r="E7" s="145"/>
-      <c r="F7" s="145"/>
-      <c r="G7" s="145"/>
+    <row r="7" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="134"/>
+      <c r="C7" s="134"/>
+      <c r="D7" s="134"/>
+      <c r="E7" s="134"/>
+      <c r="F7" s="134"/>
+      <c r="G7" s="134"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" s="6" customFormat="1" ht="15.75">
+    <row r="8" spans="1:8" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" ht="105" customHeight="1">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="9" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="10">
         <v>1</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="H11" s="14"/>
     </row>
-    <row r="12" spans="1:8" s="9" customFormat="1">
+    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="H12" s="19"/>
     </row>
-    <row r="13" spans="1:8" s="9" customFormat="1">
+    <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="H13" s="19"/>
     </row>
-    <row r="14" spans="1:8" s="9" customFormat="1">
+    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="H14" s="19"/>
     </row>
-    <row r="15" spans="1:8" s="9" customFormat="1">
+    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:8" s="9" customFormat="1">
+    <row r="16" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="H16" s="19"/>
     </row>
-    <row r="17" spans="4:8" s="9" customFormat="1" ht="14.25" customHeight="1">
+    <row r="17" spans="4:8" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="4:8" s="9" customFormat="1">
+    <row r="18" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="4:8" s="9" customFormat="1">
+    <row r="19" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="4:8" s="9" customFormat="1">
+    <row r="20" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H20" s="20"/>
     </row>
-    <row r="21" spans="4:8" s="9" customFormat="1">
+    <row r="21" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H21" s="20"/>
     </row>
-    <row r="22" spans="4:8" s="9" customFormat="1">
+    <row r="22" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H22" s="20"/>
     </row>
-    <row r="23" spans="4:8" s="9" customFormat="1">
+    <row r="23" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H23" s="20"/>
     </row>
-    <row r="24" spans="4:8" s="9" customFormat="1">
+    <row r="24" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H24" s="20"/>
     </row>
-    <row r="25" spans="4:8" s="9" customFormat="1">
+    <row r="25" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H25" s="20"/>
     </row>
-    <row r="26" spans="4:8" s="9" customFormat="1">
+    <row r="26" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H26" s="20"/>
     </row>
-    <row r="27" spans="4:8" s="9" customFormat="1">
+    <row r="27" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H27" s="20"/>
     </row>
-    <row r="28" spans="4:8" s="9" customFormat="1">
+    <row r="28" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H28" s="20"/>
     </row>
-    <row r="29" spans="4:8" s="9" customFormat="1">
+    <row r="29" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H29" s="20"/>
     </row>
-    <row r="30" spans="4:8" s="9" customFormat="1">
+    <row r="30" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H30" s="20"/>
     </row>
-    <row r="31" spans="4:8" s="9" customFormat="1">
+    <row r="31" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H31" s="20"/>
     </row>
-    <row r="32" spans="4:8" s="9" customFormat="1">
+    <row r="32" spans="4:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H32" s="20"/>
     </row>
-    <row r="33" spans="8:8" s="9" customFormat="1">
+    <row r="33" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H33" s="20"/>
     </row>
-    <row r="34" spans="8:8" s="9" customFormat="1">
+    <row r="34" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H34" s="20"/>
     </row>
-    <row r="35" spans="8:8" s="9" customFormat="1">
+    <row r="35" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H35" s="20"/>
     </row>
-    <row r="36" spans="8:8" s="9" customFormat="1">
+    <row r="36" spans="8:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H36" s="20"/>
     </row>
   </sheetData>
@@ -4386,7 +4387,7 @@
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="1"/>
     <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
@@ -4404,23 +4405,23 @@
     <col min="14" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
     </row>
-    <row r="2" spans="1:13" ht="23.25">
+    <row r="2" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="24" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="I2" s="24"/>
       <c r="J2" s="13"/>
@@ -4428,7 +4429,7 @@
       <c r="L2" s="13"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75">
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -4443,69 +4444,69 @@
       <c r="L3" s="13"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75">
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="B4" s="131" t="s">
-        <v>153</v>
-      </c>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="133"/>
+      <c r="B4" s="135" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="136"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="137"/>
       <c r="I4" s="40"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:13" ht="15.75">
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="134"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="135"/>
+      <c r="B5" s="138"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="139"/>
       <c r="I5" s="40"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75">
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="134"/>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="135"/>
+      <c r="B6" s="138"/>
+      <c r="C6" s="130"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
+      <c r="H6" s="139"/>
       <c r="I6" s="40"/>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:13" ht="15.75">
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="136"/>
-      <c r="C7" s="137"/>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="137"/>
-      <c r="G7" s="137"/>
-      <c r="H7" s="138"/>
+      <c r="B7" s="140"/>
+      <c r="C7" s="141"/>
+      <c r="D7" s="141"/>
+      <c r="E7" s="141"/>
+      <c r="F7" s="141"/>
+      <c r="G7" s="141"/>
+      <c r="H7" s="142"/>
       <c r="I7" s="40"/>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75">
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="16"/>
       <c r="C8" s="6"/>
@@ -4520,1002 +4521,1002 @@
       <c r="L8" s="13"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="26.25">
+    <row r="10" spans="1:13" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B10" s="115" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="116" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="116" t="s">
+        <v>149</v>
+      </c>
+      <c r="E10" s="116" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" s="116" t="s">
+        <v>151</v>
+      </c>
+      <c r="G10" s="116" t="s">
+        <v>152</v>
+      </c>
+      <c r="H10" s="116" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="116" t="s">
+        <v>153</v>
+      </c>
+      <c r="J10" s="116" t="s">
         <v>154</v>
       </c>
-      <c r="C10" s="116" t="s">
-        <v>155</v>
-      </c>
-      <c r="D10" s="116" t="s">
-        <v>156</v>
-      </c>
-      <c r="E10" s="116" t="s">
-        <v>157</v>
-      </c>
-      <c r="F10" s="116" t="s">
-        <v>158</v>
-      </c>
-      <c r="G10" s="116" t="s">
-        <v>159</v>
-      </c>
-      <c r="H10" s="116" t="s">
-        <v>90</v>
-      </c>
-      <c r="I10" s="116" t="s">
-        <v>160</v>
-      </c>
-      <c r="J10" s="116" t="s">
-        <v>161</v>
-      </c>
       <c r="K10" s="99" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L10" s="99" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="M10" s="99" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="113" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C11" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D11" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E11" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F11" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G11" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H11" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I11" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="J11" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K11" s="99" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L11" s="99" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="M11" s="99" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="113" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="F12" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="G12" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="I12" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="J12" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="K12" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="L12" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="M12" s="99" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="113" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="E13" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="F13" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="G13" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="H13" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="I13" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="J13" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="K13" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="L13" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="M13" s="99" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="113" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="F14" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="G14" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="H14" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="I14" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="J14" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="K14" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="L14" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="M14" s="99" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="113" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="F15" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="G15" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="H15" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="I15" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="J15" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="K15" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="L15" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="M15" s="99" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="113" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="F16" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="G16" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="H16" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="I16" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="J16" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="K16" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="L16" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="M16" s="99" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="113" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="E17" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="F17" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="G17" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="H17" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="I17" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="J17" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="K17" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="L17" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="M17" s="99" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="113" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="E18" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="F18" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="G18" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="H18" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="I18" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="J18" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="K18" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="L18" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="M18" s="99" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="113" t="s">
+        <v>155</v>
+      </c>
+      <c r="C19" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="D19" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="E19" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="F19" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="G19" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="H19" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="I19" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="J19" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="K19" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="L19" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="M19" s="99" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="113" t="s">
+        <v>155</v>
+      </c>
+      <c r="C20" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="D20" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="E20" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="F20" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="G20" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="H20" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="I20" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="J20" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="K20" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="L20" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="M20" s="99" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="113" t="s">
+        <v>155</v>
+      </c>
+      <c r="C21" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="D21" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="E21" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="F21" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="G21" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="H21" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="I21" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="J21" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="K21" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="L21" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="M21" s="99" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="113" t="s">
+        <v>155</v>
+      </c>
+      <c r="C22" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="D22" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="F22" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="G22" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="H22" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="I22" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="J22" s="114" t="s">
+        <v>155</v>
+      </c>
+      <c r="K22" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="L22" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="M22" s="99" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B25" s="111" t="s">
+        <v>156</v>
+      </c>
+      <c r="C25" s="112" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" s="112" t="s">
+        <v>158</v>
+      </c>
+      <c r="E25" s="112" t="s">
+        <v>159</v>
+      </c>
+      <c r="F25" s="112" t="s">
+        <v>160</v>
+      </c>
+      <c r="G25" s="112" t="s">
+        <v>161</v>
+      </c>
+      <c r="H25" s="112" t="s">
         <v>162</v>
       </c>
-      <c r="C12" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="D12" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="E12" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="F12" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="G12" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="H12" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="I12" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="J12" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="K12" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="L12" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="M12" s="99" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="B13" s="113" t="s">
-        <v>162</v>
-      </c>
-      <c r="C13" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="D13" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="E13" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="F13" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="G13" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="H13" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="I13" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="J13" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="K13" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="L13" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="M13" s="99" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="B14" s="113" t="s">
-        <v>162</v>
-      </c>
-      <c r="C14" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="D14" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="E14" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="F14" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="G14" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="H14" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="I14" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="J14" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="K14" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="L14" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="M14" s="99" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="B15" s="113" t="s">
-        <v>162</v>
-      </c>
-      <c r="C15" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="D15" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="E15" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="F15" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="G15" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="H15" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="I15" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="J15" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="K15" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="L15" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="M15" s="99" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="B16" s="113" t="s">
-        <v>162</v>
-      </c>
-      <c r="C16" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="D16" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="E16" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="F16" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="G16" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="H16" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="I16" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="J16" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="K16" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="L16" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="M16" s="99" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13">
-      <c r="B17" s="113" t="s">
-        <v>162</v>
-      </c>
-      <c r="C17" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="D17" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="E17" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="F17" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="G17" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="H17" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="I17" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="J17" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="K17" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="L17" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="M17" s="99" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13">
-      <c r="B18" s="113" t="s">
-        <v>162</v>
-      </c>
-      <c r="C18" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="D18" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="E18" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="F18" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="G18" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="H18" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="I18" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="J18" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="K18" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="L18" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="M18" s="99" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13">
-      <c r="B19" s="113" t="s">
-        <v>162</v>
-      </c>
-      <c r="C19" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="D19" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="E19" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="F19" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="G19" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="H19" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="I19" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="J19" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="K19" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="L19" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="M19" s="99" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13">
-      <c r="B20" s="113" t="s">
-        <v>162</v>
-      </c>
-      <c r="C20" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="D20" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="E20" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="F20" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="G20" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="H20" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="I20" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="J20" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="K20" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="L20" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="M20" s="99" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13">
-      <c r="B21" s="113" t="s">
-        <v>162</v>
-      </c>
-      <c r="C21" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="D21" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="E21" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="F21" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="G21" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="H21" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="I21" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="J21" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="K21" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="L21" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="M21" s="99" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13">
-      <c r="B22" s="113" t="s">
-        <v>162</v>
-      </c>
-      <c r="C22" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="D22" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="E22" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="F22" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="G22" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="H22" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="I22" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="J22" s="114" t="s">
-        <v>162</v>
-      </c>
-      <c r="K22" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="L22" s="99" t="s">
-        <v>162</v>
-      </c>
-      <c r="M22" s="99" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" ht="26.25">
-      <c r="B25" s="111" t="s">
+      <c r="I25" s="112" t="s">
         <v>163</v>
       </c>
-      <c r="C25" s="112" t="s">
+      <c r="J25" s="112" t="s">
+        <v>83</v>
+      </c>
+      <c r="K25" s="112" t="s">
+        <v>153</v>
+      </c>
+      <c r="L25" s="112" t="s">
+        <v>154</v>
+      </c>
+      <c r="M25" s="123" t="s">
         <v>164</v>
       </c>
-      <c r="D25" s="112" t="s">
-        <v>165</v>
-      </c>
-      <c r="E25" s="112" t="s">
-        <v>166</v>
-      </c>
-      <c r="F25" s="112" t="s">
-        <v>167</v>
-      </c>
-      <c r="G25" s="112" t="s">
-        <v>168</v>
-      </c>
-      <c r="H25" s="112" t="s">
-        <v>169</v>
-      </c>
-      <c r="I25" s="112" t="s">
-        <v>170</v>
-      </c>
-      <c r="J25" s="112" t="s">
-        <v>90</v>
-      </c>
-      <c r="K25" s="112" t="s">
-        <v>160</v>
-      </c>
-      <c r="L25" s="112" t="s">
-        <v>161</v>
-      </c>
-      <c r="M25" s="123" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13">
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="113" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C26" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D26" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E26" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F26" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G26" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H26" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I26" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="J26" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K26" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L26" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="M26" s="114" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="113" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C27" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D27" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E27" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F27" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G27" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H27" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I27" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="J27" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K27" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L27" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="M27" s="114" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="113" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C28" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D28" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E28" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F28" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G28" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H28" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I28" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="J28" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K28" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L28" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="M28" s="114" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="113" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C29" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D29" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E29" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F29" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G29" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H29" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I29" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="J29" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K29" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L29" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="M29" s="114" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="113" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C30" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D30" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E30" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F30" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G30" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H30" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I30" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="J30" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K30" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L30" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="M30" s="114" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="113" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C31" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D31" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E31" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F31" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G31" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H31" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I31" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="J31" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K31" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L31" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="M31" s="114" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="113" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C32" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D32" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E32" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F32" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G32" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H32" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I32" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="J32" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K32" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L32" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="M32" s="114" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="113" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C33" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D33" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E33" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F33" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G33" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H33" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I33" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="J33" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K33" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L33" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="M33" s="114" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="113" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C34" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D34" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E34" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F34" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G34" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H34" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I34" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="J34" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K34" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L34" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="M34" s="114" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="35" spans="2:13">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="113" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C35" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D35" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E35" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F35" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G35" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H35" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I35" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="J35" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K35" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L35" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="M35" s="114" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="113" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C36" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D36" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E36" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F36" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G36" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H36" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I36" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="J36" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K36" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L36" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="M36" s="114" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="37" spans="2:13">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="113" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C37" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D37" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E37" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F37" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G37" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="H37" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I37" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="J37" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K37" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L37" s="114" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="M37" s="114" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="40" spans="2:13">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="120"/>
       <c r="C40" s="120"/>
       <c r="D40" s="120"/>
@@ -5529,7 +5530,7 @@
       <c r="L40" s="120"/>
       <c r="M40" s="121"/>
     </row>
-    <row r="41" spans="2:13">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="122"/>
       <c r="C41" s="122"/>
       <c r="D41" s="122"/>
@@ -5543,7 +5544,7 @@
       <c r="L41" s="122"/>
       <c r="M41" s="122"/>
     </row>
-    <row r="42" spans="2:13">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="122"/>
       <c r="C42" s="122"/>
       <c r="D42" s="122"/>
@@ -5557,7 +5558,7 @@
       <c r="L42" s="122"/>
       <c r="M42" s="122"/>
     </row>
-    <row r="43" spans="2:13">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="122"/>
       <c r="C43" s="122"/>
       <c r="D43" s="122"/>
@@ -5571,7 +5572,7 @@
       <c r="L43" s="122"/>
       <c r="M43" s="122"/>
     </row>
-    <row r="44" spans="2:13">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="122"/>
       <c r="C44" s="122"/>
       <c r="D44" s="122"/>
@@ -5585,7 +5586,7 @@
       <c r="L44" s="122"/>
       <c r="M44" s="122"/>
     </row>
-    <row r="45" spans="2:13">
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" s="122"/>
       <c r="C45" s="122"/>
       <c r="D45" s="122"/>
@@ -5599,7 +5600,7 @@
       <c r="L45" s="122"/>
       <c r="M45" s="122"/>
     </row>
-    <row r="46" spans="2:13">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" s="122"/>
       <c r="C46" s="122"/>
       <c r="D46" s="122"/>
@@ -5613,7 +5614,7 @@
       <c r="L46" s="122"/>
       <c r="M46" s="122"/>
     </row>
-    <row r="47" spans="2:13">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" s="122"/>
       <c r="C47" s="122"/>
       <c r="D47" s="122"/>
@@ -5627,7 +5628,7 @@
       <c r="L47" s="122"/>
       <c r="M47" s="122"/>
     </row>
-    <row r="48" spans="2:13">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="122"/>
       <c r="C48" s="122"/>
       <c r="D48" s="122"/>
@@ -5641,7 +5642,7 @@
       <c r="L48" s="122"/>
       <c r="M48" s="122"/>
     </row>
-    <row r="49" spans="2:13">
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49" s="122"/>
       <c r="C49" s="122"/>
       <c r="D49" s="122"/>
@@ -5655,7 +5656,7 @@
       <c r="L49" s="122"/>
       <c r="M49" s="122"/>
     </row>
-    <row r="50" spans="2:13">
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B50" s="122"/>
       <c r="C50" s="122"/>
       <c r="D50" s="122"/>
@@ -5669,7 +5670,7 @@
       <c r="L50" s="122"/>
       <c r="M50" s="122"/>
     </row>
-    <row r="51" spans="2:13">
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B51" s="122"/>
       <c r="C51" s="122"/>
       <c r="D51" s="122"/>
@@ -5683,7 +5684,7 @@
       <c r="L51" s="122"/>
       <c r="M51" s="122"/>
     </row>
-    <row r="52" spans="2:13">
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52" s="122"/>
       <c r="C52" s="122"/>
       <c r="D52" s="122"/>
@@ -5739,7 +5740,7 @@
       <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
@@ -5760,12 +5761,12 @@
     <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" s="6" customFormat="1" ht="23.25">
+    <row r="2" spans="1:20" s="6" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="D2" s="7" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
@@ -5774,7 +5775,7 @@
       <c r="O2" s="13"/>
       <c r="P2" s="13"/>
     </row>
-    <row r="3" spans="1:20" s="6" customFormat="1" ht="15.75">
+    <row r="3" spans="1:20" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
@@ -5782,18 +5783,18 @@
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
     </row>
-    <row r="4" spans="1:20" s="6" customFormat="1" ht="15.75">
-      <c r="B4" s="144" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4" s="144"/>
-      <c r="D4" s="145"/>
-      <c r="E4" s="145"/>
-      <c r="F4" s="145"/>
-      <c r="G4" s="145"/>
-      <c r="H4" s="145"/>
-      <c r="I4" s="145"/>
-      <c r="J4" s="145"/>
+    <row r="4" spans="1:20" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="133" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="133"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="134"/>
+      <c r="F4" s="134"/>
+      <c r="G4" s="134"/>
+      <c r="H4" s="134"/>
+      <c r="I4" s="134"/>
+      <c r="J4" s="134"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
@@ -5801,16 +5802,16 @@
       <c r="O4" s="13"/>
       <c r="P4" s="13"/>
     </row>
-    <row r="5" spans="1:20" s="6" customFormat="1" ht="15.75">
-      <c r="B5" s="145"/>
-      <c r="C5" s="145"/>
-      <c r="D5" s="145"/>
-      <c r="E5" s="145"/>
-      <c r="F5" s="145"/>
-      <c r="G5" s="145"/>
-      <c r="H5" s="145"/>
-      <c r="I5" s="145"/>
-      <c r="J5" s="145"/>
+    <row r="5" spans="1:20" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="134"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
@@ -5818,16 +5819,16 @@
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
     </row>
-    <row r="6" spans="1:20" s="6" customFormat="1" ht="15.75">
-      <c r="B6" s="145"/>
-      <c r="C6" s="145"/>
-      <c r="D6" s="145"/>
-      <c r="E6" s="145"/>
-      <c r="F6" s="145"/>
-      <c r="G6" s="145"/>
-      <c r="H6" s="145"/>
-      <c r="I6" s="145"/>
-      <c r="J6" s="145"/>
+    <row r="6" spans="1:20" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="134"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
@@ -5835,16 +5836,16 @@
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
     </row>
-    <row r="7" spans="1:20" s="6" customFormat="1" ht="15.75">
-      <c r="B7" s="145"/>
-      <c r="C7" s="145"/>
-      <c r="D7" s="145"/>
-      <c r="E7" s="145"/>
-      <c r="F7" s="145"/>
-      <c r="G7" s="145"/>
-      <c r="H7" s="145"/>
-      <c r="I7" s="145"/>
-      <c r="J7" s="145"/>
+    <row r="7" spans="1:20" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="134"/>
+      <c r="C7" s="134"/>
+      <c r="D7" s="134"/>
+      <c r="E7" s="134"/>
+      <c r="F7" s="134"/>
+      <c r="G7" s="134"/>
+      <c r="H7" s="134"/>
+      <c r="I7" s="134"/>
+      <c r="J7" s="134"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
@@ -5852,18 +5853,18 @@
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
-    <row r="8" spans="1:20" s="6" customFormat="1" ht="15.75">
-      <c r="B8" s="146" t="s">
-        <v>174</v>
-      </c>
-      <c r="C8" s="147"/>
-      <c r="D8" s="146"/>
-      <c r="E8" s="146"/>
-      <c r="F8" s="146"/>
-      <c r="G8" s="146"/>
-      <c r="H8" s="146"/>
-      <c r="I8" s="146"/>
-      <c r="J8" s="146"/>
+    <row r="8" spans="1:20" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="125" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="126"/>
+      <c r="D8" s="125"/>
+      <c r="E8" s="125"/>
+      <c r="F8" s="125"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="125"/>
+      <c r="J8" s="125"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
@@ -5871,66 +5872,66 @@
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
     </row>
-    <row r="10" spans="1:20" ht="36">
+    <row r="10" spans="1:20" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="K10" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="L10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="M10" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="N10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O10" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="P10" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="Q10" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="R10" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="S10" s="86" t="s">
         <v>182</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="T10" s="86" t="s">
         <v>183</v>
       </c>
-      <c r="K10" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="O10" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="P10" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q10" s="84" t="s">
-        <v>92</v>
-      </c>
-      <c r="R10" s="86" t="s">
-        <v>188</v>
-      </c>
-      <c r="S10" s="86" t="s">
-        <v>189</v>
-      </c>
-      <c r="T10" s="86" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" s="9" customFormat="1" ht="105" customHeight="1">
+    </row>
+    <row r="11" spans="1:20" s="9" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="15">
         <v>1</v>
@@ -5951,16 +5952,16 @@
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
       <c r="R11" s="85" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="S11" s="87" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="T11" s="87" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" s="9" customFormat="1">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
@@ -5975,7 +5976,7 @@
       <c r="P12" s="20"/>
       <c r="Q12" s="22"/>
     </row>
-    <row r="13" spans="1:20" s="9" customFormat="1">
+    <row r="13" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
@@ -5990,7 +5991,7 @@
       <c r="P13" s="20"/>
       <c r="Q13" s="22"/>
     </row>
-    <row r="14" spans="1:20" s="9" customFormat="1">
+    <row r="14" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
@@ -6005,7 +6006,7 @@
       <c r="P14" s="20"/>
       <c r="Q14" s="21"/>
     </row>
-    <row r="15" spans="1:20" s="9" customFormat="1">
+    <row r="15" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
@@ -6020,7 +6021,7 @@
       <c r="P15" s="20"/>
       <c r="Q15" s="21"/>
     </row>
-    <row r="16" spans="1:20" s="9" customFormat="1">
+    <row r="16" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
@@ -6035,7 +6036,7 @@
       <c r="P16" s="20"/>
       <c r="Q16" s="21"/>
     </row>
-    <row r="17" spans="4:17" s="9" customFormat="1" ht="14.25" customHeight="1">
+    <row r="17" spans="4:17" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
@@ -6050,7 +6051,7 @@
       <c r="P17" s="20"/>
       <c r="Q17" s="21"/>
     </row>
-    <row r="18" spans="4:17" s="9" customFormat="1">
+    <row r="18" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
@@ -6065,7 +6066,7 @@
       <c r="P18" s="20"/>
       <c r="Q18" s="21"/>
     </row>
-    <row r="19" spans="4:17" s="9" customFormat="1">
+    <row r="19" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K19" s="20"/>
       <c r="L19" s="20"/>
       <c r="M19" s="20"/>
@@ -6074,7 +6075,7 @@
       <c r="P19" s="20"/>
       <c r="Q19" s="22"/>
     </row>
-    <row r="20" spans="4:17" s="9" customFormat="1">
+    <row r="20" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
@@ -6083,7 +6084,7 @@
       <c r="P20" s="20"/>
       <c r="Q20" s="22"/>
     </row>
-    <row r="21" spans="4:17" s="9" customFormat="1">
+    <row r="21" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
@@ -6092,7 +6093,7 @@
       <c r="P21" s="20"/>
       <c r="Q21" s="22"/>
     </row>
-    <row r="22" spans="4:17" s="9" customFormat="1">
+    <row r="22" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
@@ -6101,7 +6102,7 @@
       <c r="P22" s="20"/>
       <c r="Q22" s="22"/>
     </row>
-    <row r="23" spans="4:17" s="9" customFormat="1">
+    <row r="23" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
       <c r="M23" s="20"/>
@@ -6110,7 +6111,7 @@
       <c r="P23" s="20"/>
       <c r="Q23" s="22"/>
     </row>
-    <row r="24" spans="4:17" s="9" customFormat="1">
+    <row r="24" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
@@ -6119,7 +6120,7 @@
       <c r="P24" s="20"/>
       <c r="Q24" s="22"/>
     </row>
-    <row r="25" spans="4:17" s="9" customFormat="1">
+    <row r="25" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K25" s="20"/>
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
@@ -6128,7 +6129,7 @@
       <c r="P25" s="20"/>
       <c r="Q25" s="22"/>
     </row>
-    <row r="26" spans="4:17" s="9" customFormat="1">
+    <row r="26" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
@@ -6137,7 +6138,7 @@
       <c r="P26" s="20"/>
       <c r="Q26" s="22"/>
     </row>
-    <row r="27" spans="4:17" s="9" customFormat="1">
+    <row r="27" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K27" s="20"/>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
@@ -6146,7 +6147,7 @@
       <c r="P27" s="20"/>
       <c r="Q27" s="22"/>
     </row>
-    <row r="28" spans="4:17" s="9" customFormat="1">
+    <row r="28" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K28" s="20"/>
       <c r="L28" s="20"/>
       <c r="M28" s="20"/>
@@ -6155,7 +6156,7 @@
       <c r="P28" s="20"/>
       <c r="Q28" s="22"/>
     </row>
-    <row r="29" spans="4:17" s="9" customFormat="1">
+    <row r="29" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K29" s="20"/>
       <c r="L29" s="20"/>
       <c r="M29" s="20"/>
@@ -6164,7 +6165,7 @@
       <c r="P29" s="20"/>
       <c r="Q29" s="22"/>
     </row>
-    <row r="30" spans="4:17" s="9" customFormat="1">
+    <row r="30" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K30" s="20"/>
       <c r="L30" s="20"/>
       <c r="M30" s="20"/>
@@ -6173,7 +6174,7 @@
       <c r="P30" s="20"/>
       <c r="Q30" s="22"/>
     </row>
-    <row r="31" spans="4:17" s="9" customFormat="1">
+    <row r="31" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K31" s="20"/>
       <c r="L31" s="20"/>
       <c r="M31" s="20"/>
@@ -6182,7 +6183,7 @@
       <c r="P31" s="20"/>
       <c r="Q31" s="22"/>
     </row>
-    <row r="32" spans="4:17" s="9" customFormat="1">
+    <row r="32" spans="4:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
       <c r="M32" s="20"/>
@@ -6191,7 +6192,7 @@
       <c r="P32" s="20"/>
       <c r="Q32" s="22"/>
     </row>
-    <row r="33" spans="11:17" s="9" customFormat="1">
+    <row r="33" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K33" s="20"/>
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
@@ -6200,7 +6201,7 @@
       <c r="P33" s="20"/>
       <c r="Q33" s="22"/>
     </row>
-    <row r="34" spans="11:17" s="9" customFormat="1">
+    <row r="34" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
       <c r="M34" s="20"/>
@@ -6209,7 +6210,7 @@
       <c r="P34" s="20"/>
       <c r="Q34" s="22"/>
     </row>
-    <row r="35" spans="11:17" s="9" customFormat="1">
+    <row r="35" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
       <c r="M35" s="20"/>
@@ -6218,7 +6219,7 @@
       <c r="P35" s="20"/>
       <c r="Q35" s="22"/>
     </row>
-    <row r="36" spans="11:17" s="9" customFormat="1">
+    <row r="36" spans="11:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="K36" s="20"/>
       <c r="L36" s="20"/>
       <c r="M36" s="20"/>
@@ -6267,7 +6268,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="30" style="1" customWidth="1"/>
@@ -6280,81 +6281,81 @@
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="138.75" customHeight="1">
+    <row r="2" spans="1:8" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="139" t="s">
+      <c r="B2" s="143" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="109" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F2" s="146" t="s">
+        <v>189</v>
+      </c>
+      <c r="G2" s="110" t="s">
+        <v>186</v>
+      </c>
+      <c r="H2" s="83" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="108" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="147"/>
+      <c r="G3" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="H3" s="83" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="109" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="4" t="s">
+    </row>
+    <row r="4" spans="1:8" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="145"/>
+      <c r="C4" s="107" t="s">
         <v>195</v>
       </c>
-      <c r="F2" s="142" t="s">
+      <c r="D4" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="G2" s="110" t="s">
-        <v>193</v>
-      </c>
-      <c r="H2" s="83" t="s">
+      <c r="F4" s="147"/>
+      <c r="G4" s="110" t="s">
+        <v>185</v>
+      </c>
+      <c r="H4" s="83" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="144.75" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="140"/>
-      <c r="C3" s="108" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="110" t="s">
-        <v>200</v>
-      </c>
-      <c r="H3" s="83" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="121.5" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="141"/>
-      <c r="C4" s="107" t="s">
-        <v>202</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="F4" s="143"/>
-      <c r="G4" s="110" t="s">
-        <v>192</v>
-      </c>
-      <c r="H4" s="83" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="F7" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
     </row>
   </sheetData>
@@ -6371,26 +6372,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e1cd103-0302-4a32-9a4b-e115c950d959">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031C6D98A8BA9914F9CBD1D8D43561C2B" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="20dc68b959a60313fbcac393e99fd10f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e1cd103-0302-4a32-9a4b-e115c950d959" xmlns:ns3="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7195712bd1d9adc40779bc7b93adecf4" ns2:_="" ns3:_="">
     <xsd:import namespace="7e1cd103-0302-4a32-9a4b-e115c950d959"/>
@@ -6633,14 +6614,60 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e1cd103-0302-4a32-9a4b-e115c950d959">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71C399E-D560-405D-A693-6A86DF1C82D7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8A29AC-6BF1-4D4D-9282-8A0E51881B4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7e1cd103-0302-4a32-9a4b-e115c950d959"/>
+    <ds:schemaRef ds:uri="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D186559C-C381-484C-9B7A-F4466E79AE25}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D186559C-C381-484C-9B7A-F4466E79AE25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8A29AC-6BF1-4D4D-9282-8A0E51881B4F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D71C399E-D560-405D-A693-6A86DF1C82D7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7e1cd103-0302-4a32-9a4b-e115c950d959"/>
+    <ds:schemaRef ds:uri="50b62f6a-6a2d-4510-bfe7-b1a3c00072e4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>